<commit_message>
Finished Week 8 Excel example
</commit_message>
<xml_diff>
--- a/Module 2/Week 8 - Portfolio statistics and CAPM/Homework 2 example.xlsx
+++ b/Module 2/Week 8 - Portfolio statistics and CAPM/Homework 2 example.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Excess returns" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Optimal portfolio from homework" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Data" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Excess returns" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Optimal portfolio from homework" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
   <si>
     <t xml:space="preserve">Month</t>
   </si>
@@ -162,6 +162,9 @@
     <t xml:space="preserve">SD of regression residuals, using formula in slides:</t>
   </si>
   <si>
+    <t xml:space="preserve">SD of regression residuals, calculated manually:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Information ratio of gold with respect to VFINX:</t>
   </si>
   <si>
@@ -189,7 +192,7 @@
     <numFmt numFmtId="168" formatCode="General"/>
     <numFmt numFmtId="169" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -227,12 +230,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -289,55 +286,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,8 +350,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3085,21 +3188,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:N193"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A171" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="18.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="17.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.77"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.52"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
@@ -3115,22 +3218,22 @@
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -3152,12 +3255,20 @@
       </c>
       <c r="G2" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B2 + 'Optimal portfolio from homework'!$C$15*C2</f>
-        <v>-0.00462186237345621</v>
+        <v>-0.00462186237345638</v>
       </c>
       <c r="I2" s="1" t="n">
         <f aca="false">0.5*B2+0.5*C2</f>
         <v>0.019974131618385</v>
       </c>
+      <c r="M2" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B2</f>
+        <v>0.000149613527067106</v>
+      </c>
+      <c r="N2" s="8" t="n">
+        <f aca="false">C2-M2</f>
+        <v>0.102054032617583</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -3183,6 +3294,14 @@
         <f aca="false">0.5*B3+0.5*C3</f>
         <v>0.00693527519240368</v>
       </c>
+      <c r="M3" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B3</f>
+        <v>0.00221775417529374</v>
+      </c>
+      <c r="N3" s="8" t="n">
+        <f aca="false">C3-M3</f>
+        <v>0.0454673608450041</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -3208,6 +3327,14 @@
         <f aca="false">0.5*B4+0.5*C4</f>
         <v>-0.020285357549648</v>
       </c>
+      <c r="M4" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B4</f>
+        <v>0.0042327216604046</v>
+      </c>
+      <c r="N4" s="8" t="n">
+        <f aca="false">C4-M4</f>
+        <v>-0.0386984595345016</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -3227,12 +3354,20 @@
       </c>
       <c r="G5" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B5 + 'Optimal portfolio from homework'!$C$15*C5</f>
-        <v>0.00374441605614449</v>
+        <v>0.00374441605614451</v>
       </c>
       <c r="I5" s="1" t="n">
         <f aca="false">0.5*B5+0.5*C5</f>
         <v>-0.01460550651974</v>
       </c>
+      <c r="M5" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B5</f>
+        <v>0.00807562013247252</v>
+      </c>
+      <c r="N5" s="8" t="n">
+        <f aca="false">C5-M5</f>
+        <v>-0.0840287276278046</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -3258,6 +3393,14 @@
         <f aca="false">0.5*B6+0.5*C6</f>
         <v>0.0114328616332827</v>
       </c>
+      <c r="M6" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B6</f>
+        <v>0.00548563663718468</v>
+      </c>
+      <c r="N6" s="8" t="n">
+        <f aca="false">C6-M6</f>
+        <v>0.00625512971257042</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -3283,6 +3426,14 @@
         <f aca="false">0.5*B7+0.5*C7</f>
         <v>-0.0136179746301339</v>
       </c>
+      <c r="M7" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B7</f>
+        <v>-0.00158297388126448</v>
+      </c>
+      <c r="N7" s="8" t="n">
+        <f aca="false">C7-M7</f>
+        <v>0.060428738520264</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -3308,6 +3459,14 @@
         <f aca="false">0.5*B8+0.5*C8</f>
         <v>-0.0167815567985832</v>
       </c>
+      <c r="M8" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B8</f>
+        <v>0.00396278836950239</v>
+      </c>
+      <c r="N8" s="8" t="n">
+        <f aca="false">C8-M8</f>
+        <v>-0.0277088350057929</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -3333,6 +3492,14 @@
         <f aca="false">0.5*B9+0.5*C9</f>
         <v>-0.0354610504920838</v>
       </c>
+      <c r="M9" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B9</f>
+        <v>0.00563383674412949</v>
+      </c>
+      <c r="N9" s="8" t="n">
+        <f aca="false">C9-M9</f>
+        <v>-0.0897189244634278</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -3352,12 +3519,20 @@
       </c>
       <c r="G10" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B10 + 'Optimal portfolio from homework'!$C$15*C10</f>
-        <v>-0.0340041557041742</v>
+        <v>-0.0340041557041743</v>
       </c>
       <c r="I10" s="1" t="n">
         <f aca="false">0.5*B10+0.5*C10</f>
         <v>-0.0098677732744259</v>
       </c>
+      <c r="M10" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B10</f>
+        <v>-0.00190867463016291</v>
+      </c>
+      <c r="N10" s="8" t="n">
+        <f aca="false">C10-M10</f>
+        <v>0.0727338390055364</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -3383,6 +3558,14 @@
         <f aca="false">0.5*B11+0.5*C11</f>
         <v>-0.178686192309094</v>
       </c>
+      <c r="M11" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B11</f>
+        <v>-0.00759250116777866</v>
+      </c>
+      <c r="N11" s="8" t="n">
+        <f aca="false">C11-M11</f>
+        <v>-0.181055882332778</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -3402,12 +3585,20 @@
       </c>
       <c r="G12" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B12 + 'Optimal portfolio from homework'!$C$15*C12</f>
-        <v>-0.00601562936856333</v>
+        <v>-0.00601562936856329</v>
       </c>
       <c r="I12" s="1" t="n">
         <f aca="false">0.5*B12+0.5*C12</f>
         <v>0.0221648643549224</v>
       </c>
+      <c r="M12" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B12</f>
+        <v>-0.000562506951621856</v>
+      </c>
+      <c r="N12" s="8" t="n">
+        <f aca="false">C12-M12</f>
+        <v>0.116940612648259</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
@@ -3427,12 +3618,20 @@
       </c>
       <c r="G13" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B13 + 'Optimal portfolio from homework'!$C$15*C13</f>
-        <v>0.029116870651478</v>
+        <v>0.0291168706514781</v>
       </c>
       <c r="I13" s="1" t="n">
         <f aca="false">0.5*B13+0.5*C13</f>
         <v>0.0369888933106554</v>
       </c>
+      <c r="M13" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B13</f>
+        <v>0.00545263243687891</v>
+      </c>
+      <c r="N13" s="8" t="n">
+        <f aca="false">C13-M13</f>
+        <v>0.0578540670099559</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
@@ -3452,12 +3651,20 @@
       </c>
       <c r="G14" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B14 + 'Optimal portfolio from homework'!$C$15*C14</f>
-        <v>-0.0329696000979302</v>
+        <v>-0.0329696000979303</v>
       </c>
       <c r="I14" s="1" t="n">
         <f aca="false">0.5*B14+0.5*C14</f>
         <v>-0.0111379679531284</v>
       </c>
+      <c r="M14" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B14</f>
+        <v>-0.00144073389168266</v>
+      </c>
+      <c r="N14" s="8" t="n">
+        <f aca="false">C14-M14</f>
+        <v>0.0632904448743417</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
@@ -3477,12 +3684,20 @@
       </c>
       <c r="G15" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B15 + 'Optimal portfolio from homework'!$C$15*C15</f>
-        <v>-0.0596896376799625</v>
+        <v>-0.0596896376799627</v>
       </c>
       <c r="I15" s="1" t="n">
         <f aca="false">0.5*B15+0.5*C15</f>
         <v>-0.0396399143178224</v>
       </c>
+      <c r="M15" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B15</f>
+        <v>-0.00308012125644394</v>
+      </c>
+      <c r="N15" s="8" t="n">
+        <f aca="false">C15-M15</f>
+        <v>0.0304705948547019</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
@@ -3502,12 +3717,20 @@
       </c>
       <c r="G16" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B16 + 'Optimal portfolio from homework'!$C$15*C16</f>
-        <v>0.0473253861406638</v>
+        <v>0.0473253861406639</v>
       </c>
       <c r="I16" s="1" t="n">
         <f aca="false">0.5*B16+0.5*C16</f>
         <v>0.0302227376989683</v>
       </c>
+      <c r="M16" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B16</f>
+        <v>0.0110321870297605</v>
+      </c>
+      <c r="N16" s="8" t="n">
+        <f aca="false">C16-M16</f>
+        <v>-0.0379871539171777</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
@@ -3533,6 +3756,14 @@
         <f aca="false">0.5*B17+0.5*C17</f>
         <v>0.0316353261391655</v>
       </c>
+      <c r="M17" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B17</f>
+        <v>0.0116203098227008</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <f aca="false">C17-M17</f>
+        <v>-0.0438378928384874</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
@@ -3552,12 +3783,20 @@
       </c>
       <c r="G18" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B18 + 'Optimal portfolio from homework'!$C$15*C18</f>
-        <v>0.0692086785688376</v>
+        <v>0.0692086785688375</v>
       </c>
       <c r="I18" s="1" t="n">
         <f aca="false">0.5*B18+0.5*C18</f>
         <v>0.0747701559676406</v>
       </c>
+      <c r="M18" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B18</f>
+        <v>0.00876170008212539</v>
+      </c>
+      <c r="N18" s="8" t="n">
+        <f aca="false">C18-M18</f>
+        <v>0.0846016295016767</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
@@ -3577,12 +3816,20 @@
       </c>
       <c r="G19" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B19 + 'Optimal portfolio from homework'!$C$15*C19</f>
-        <v>-0.00984791446374182</v>
+        <v>-0.0098479144637418</v>
       </c>
       <c r="I19" s="1" t="n">
         <f aca="false">0.5*B19+0.5*C19</f>
         <v>-0.0149467012570139</v>
       </c>
+      <c r="M19" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B19</f>
+        <v>0.00482933680733675</v>
+      </c>
+      <c r="N19" s="8" t="n">
+        <f aca="false">C19-M19</f>
+        <v>-0.0368223409225631</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
@@ -3602,12 +3849,20 @@
       </c>
       <c r="G20" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B20 + 'Optimal portfolio from homework'!$C$15*C20</f>
-        <v>0.0474469315478233</v>
+        <v>0.0474469315478234</v>
       </c>
       <c r="I20" s="1" t="n">
         <f aca="false">0.5*B20+0.5*C20</f>
         <v>0.0353984450873491</v>
       </c>
+      <c r="M20" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B20</f>
+        <v>0.0101798376054158</v>
+      </c>
+      <c r="N20" s="8" t="n">
+        <f aca="false">C20-M20</f>
+        <v>-0.0150619842579131</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
@@ -3633,6 +3888,14 @@
         <f aca="false">0.5*B21+0.5*C21</f>
         <v>0.0255024098150015</v>
       </c>
+      <c r="M21" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B21</f>
+        <v>0.00728638208639568</v>
+      </c>
+      <c r="N21" s="8" t="n">
+        <f aca="false">C21-M21</f>
+        <v>0.00782984855962672</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
@@ -3652,12 +3915,20 @@
       </c>
       <c r="G22" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B22 + 'Optimal portfolio from homework'!$C$15*C22</f>
-        <v>0.0426567842095315</v>
+        <v>0.0426567842095316</v>
       </c>
       <c r="I22" s="1" t="n">
         <f aca="false">0.5*B22+0.5*C22</f>
         <v>0.0450419285040312</v>
       </c>
+      <c r="M22" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B22</f>
+        <v>0.00737213815000445</v>
+      </c>
+      <c r="N22" s="8" t="n">
+        <f aca="false">C22-M22</f>
+        <v>0.0456438229333507</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
@@ -3677,12 +3948,20 @@
       </c>
       <c r="G23" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B23 + 'Optimal portfolio from homework'!$C$15*C23</f>
-        <v>0.0030064542933111</v>
+        <v>0.00300645429331112</v>
       </c>
       <c r="I23" s="1" t="n">
         <f aca="false">0.5*B23+0.5*C23</f>
         <v>0.0122598803829743</v>
       </c>
+      <c r="M23" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B23</f>
+        <v>0.00331857256529759</v>
+      </c>
+      <c r="N23" s="8" t="n">
+        <f aca="false">C23-M23</f>
+        <v>0.0398774324284603</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
@@ -3702,12 +3981,20 @@
       </c>
       <c r="G24" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B24 + 'Optimal portfolio from homework'!$C$15*C24</f>
-        <v>0.0816303846189443</v>
+        <v>0.0816303846189444</v>
       </c>
       <c r="I24" s="1" t="n">
         <f aca="false">0.5*B24+0.5*C24</f>
         <v>0.0909409205246785</v>
       </c>
+      <c r="M24" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B24</f>
+        <v>0.00902616458218526</v>
+      </c>
+      <c r="N24" s="8" t="n">
+        <f aca="false">C24-M24</f>
+        <v>0.113041810525522</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
@@ -3727,12 +4014,20 @@
       </c>
       <c r="G25" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B25 + 'Optimal portfolio from homework'!$C$15*C25</f>
-        <v>-0.00779574844581269</v>
+        <v>-0.00779574844581267</v>
       </c>
       <c r="I25" s="1" t="n">
         <f aca="false">0.5*B25+0.5*C25</f>
         <v>-0.0193827444582209</v>
       </c>
+      <c r="M25" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B25</f>
+        <v>0.00608410266991583</v>
+      </c>
+      <c r="N25" s="8" t="n">
+        <f aca="false">C25-M25</f>
+        <v>-0.0642045804856154</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="n">
@@ -3758,6 +4053,14 @@
         <f aca="false">0.5*B26+0.5*C26</f>
         <v>-0.0276429896933048</v>
       </c>
+      <c r="M26" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B26</f>
+        <v>0.00205608706955395</v>
+      </c>
+      <c r="N26" s="8" t="n">
+        <f aca="false">C26-M26</f>
+        <v>-0.021304275475351</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="n">
@@ -3777,12 +4080,20 @@
       </c>
       <c r="G27" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B27 + 'Optimal portfolio from homework'!$C$15*C27</f>
-        <v>0.0297121908171083</v>
+        <v>0.0297121908171084</v>
       </c>
       <c r="I27" s="1" t="n">
         <f aca="false">0.5*B27+0.5*C27</f>
         <v>0.029197396774867</v>
       </c>
+      <c r="M27" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B27</f>
+        <v>0.00692496753805602</v>
+      </c>
+      <c r="N27" s="8" t="n">
+        <f aca="false">C27-M27</f>
+        <v>0.0205513658722419</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="n">
@@ -3808,6 +4119,14 @@
         <f aca="false">0.5*B28+0.5*C28</f>
         <v>0.0286194358115937</v>
       </c>
+      <c r="M28" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B28</f>
+        <v>0.00904228128217143</v>
+      </c>
+      <c r="N28" s="8" t="n">
+        <f aca="false">C28-M28</f>
+        <v>-0.0118389104956546</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="n">
@@ -3827,12 +4146,20 @@
       </c>
       <c r="G29" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B29 + 'Optimal portfolio from homework'!$C$15*C29</f>
-        <v>0.030917712506102</v>
+        <v>0.0309177125061019</v>
       </c>
       <c r="I29" s="1" t="n">
         <f aca="false">0.5*B29+0.5*C29</f>
         <v>0.0374205597824448</v>
       </c>
+      <c r="M29" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B29</f>
+        <v>0.00581688115806618</v>
+      </c>
+      <c r="N29" s="8" t="n">
+        <f aca="false">C29-M29</f>
+        <v>0.0533440471880357</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="n">
@@ -3858,6 +4185,14 @@
         <f aca="false">0.5*B30+0.5*C30</f>
         <v>-0.0236397330597259</v>
       </c>
+      <c r="M30" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B30</f>
+        <v>-0.00115172081524307</v>
+      </c>
+      <c r="N30" s="8" t="n">
+        <f aca="false">C30-M30</f>
+        <v>0.0340234289624458</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="n">
@@ -3877,12 +4212,20 @@
       </c>
       <c r="G31" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B31 + 'Optimal portfolio from homework'!$C$15*C31</f>
-        <v>-0.0264835533807631</v>
+        <v>-0.0264835533807632</v>
       </c>
       <c r="I31" s="1" t="n">
         <f aca="false">0.5*B31+0.5*C31</f>
         <v>-0.015382951436002</v>
       </c>
+      <c r="M31" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B31</f>
+        <v>0.000859393990016984</v>
+      </c>
+      <c r="N31" s="8" t="n">
+        <f aca="false">C31-M31</f>
+        <v>0.020869271578352</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
@@ -3908,6 +4251,14 @@
         <f aca="false">0.5*B32+0.5*C32</f>
         <v>0.00565841998174642</v>
       </c>
+      <c r="M32" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B32</f>
+        <v>0.00975676658572677</v>
+      </c>
+      <c r="N32" s="8" t="n">
+        <f aca="false">C32-M32</f>
+        <v>-0.0683009423213173</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
@@ -3927,12 +4278,20 @@
       </c>
       <c r="G33" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B33 + 'Optimal portfolio from homework'!$C$15*C33</f>
-        <v>-0.00987114238946018</v>
+        <v>-0.0098711423894602</v>
       </c>
       <c r="I33" s="1" t="n">
         <f aca="false">0.5*B33+0.5*C33</f>
         <v>0.00529044215347051</v>
       </c>
+      <c r="M33" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B33</f>
+        <v>0.00137544609042308</v>
+      </c>
+      <c r="N33" s="8" t="n">
+        <f aca="false">C33-M33</f>
+        <v>0.0546033210328645</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
@@ -3952,12 +4311,20 @@
       </c>
       <c r="G34" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B34 + 'Optimal portfolio from homework'!$C$15*C34</f>
-        <v>0.0798514169259404</v>
+        <v>0.0798514169259403</v>
       </c>
       <c r="I34" s="1" t="n">
         <f aca="false">0.5*B34+0.5*C34</f>
         <v>0.075909153271998</v>
       </c>
+      <c r="M34" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B34</f>
+        <v>0.0111549714850859</v>
+      </c>
+      <c r="N34" s="8" t="n">
+        <f aca="false">C34-M34</f>
+        <v>0.0515743759004025</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="n">
@@ -3983,6 +4350,14 @@
         <f aca="false">0.5*B35+0.5*C35</f>
         <v>0.0286623047263829</v>
       </c>
+      <c r="M35" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B35</f>
+        <v>0.00742414693573317</v>
+      </c>
+      <c r="N35" s="8" t="n">
+        <f aca="false">C35-M35</f>
+        <v>0.0121173481062196</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
@@ -4002,12 +4377,20 @@
       </c>
       <c r="G36" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B36 + 'Optimal portfolio from homework'!$C$15*C36</f>
-        <v>0.00992763861355076</v>
+        <v>0.00992763861355075</v>
       </c>
       <c r="I36" s="1" t="n">
         <f aca="false">0.5*B36+0.5*C36</f>
         <v>0.0142070880867776</v>
       </c>
+      <c r="M36" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B36</f>
+        <v>0.0046693876301445</v>
+      </c>
+      <c r="N36" s="8" t="n">
+        <f aca="false">C36-M36</f>
+        <v>0.0238447885434107</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
@@ -4033,6 +4416,14 @@
         <f aca="false">0.5*B37+0.5*C37</f>
         <v>0.0460748715306687</v>
       </c>
+      <c r="M37" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B37</f>
+        <v>0.00952060711503876</v>
+      </c>
+      <c r="N37" s="8" t="n">
+        <f aca="false">C37-M37</f>
+        <v>0.0160157565213249</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="n">
@@ -4052,12 +4443,20 @@
       </c>
       <c r="G38" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B38 + 'Optimal portfolio from homework'!$C$15*C38</f>
-        <v>-0.00386140681263684</v>
+        <v>-0.0038614068126368</v>
       </c>
       <c r="I38" s="1" t="n">
         <f aca="false">0.5*B38+0.5*C38</f>
         <v>-0.0155259580553862</v>
       </c>
+      <c r="M38" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B38</f>
+        <v>0.00638341230480699</v>
+      </c>
+      <c r="N38" s="8" t="n">
+        <f aca="false">C38-M38</f>
+        <v>-0.0609063869546918</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="n">
@@ -4083,6 +4482,14 @@
         <f aca="false">0.5*B39+0.5*C39</f>
         <v>0.0455715764810294</v>
       </c>
+      <c r="M39" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B39</f>
+        <v>0.00715361560513722</v>
+      </c>
+      <c r="N39" s="8" t="n">
+        <f aca="false">C39-M39</f>
+        <v>0.0499267368508059</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="n">
@@ -4108,6 +4515,14 @@
         <f aca="false">0.5*B40+0.5*C40</f>
         <v>0.00756488559037082</v>
       </c>
+      <c r="M40" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B40</f>
+        <v>0.0046880161089781</v>
+      </c>
+      <c r="N40" s="8" t="n">
+        <f aca="false">C40-M40</f>
+        <v>0.0102855784999952</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="n">
@@ -4133,6 +4548,14 @@
         <f aca="false">0.5*B41+0.5*C41</f>
         <v>0.0496802013713928</v>
       </c>
+      <c r="M41" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B41</f>
+        <v>0.00682030842651282</v>
+      </c>
+      <c r="N41" s="8" t="n">
+        <f aca="false">C41-M41</f>
+        <v>0.0630608935301609</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
@@ -4158,6 +4581,14 @@
         <f aca="false">0.5*B42+0.5*C42</f>
         <v>-0.0037675088161036</v>
       </c>
+      <c r="M42" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B42</f>
+        <v>0.00384375314873724</v>
+      </c>
+      <c r="N42" s="8" t="n">
+        <f aca="false">C42-M42</f>
+        <v>7.52540361092582E-005</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
@@ -4183,6 +4614,14 @@
         <f aca="false">0.5*B43+0.5*C43</f>
         <v>-0.0177953585288541</v>
       </c>
+      <c r="M43" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B43</f>
+        <v>0.00346062237635161</v>
+      </c>
+      <c r="N43" s="8" t="n">
+        <f aca="false">C43-M43</f>
+        <v>-0.0223285469046535</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
@@ -4202,12 +4641,20 @@
       </c>
       <c r="G44" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B44 + 'Optimal portfolio from homework'!$C$15*C44</f>
-        <v>0.0112796720242083</v>
+        <v>0.0112796720242082</v>
       </c>
       <c r="I44" s="1" t="n">
         <f aca="false">0.5*B44+0.5*C44</f>
         <v>0.0248287186791693</v>
       </c>
+      <c r="M44" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B44</f>
+        <v>0.00318824032382749</v>
+      </c>
+      <c r="N44" s="8" t="n">
+        <f aca="false">C44-M44</f>
+        <v>0.0669377543711327</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
@@ -4233,6 +4680,14 @@
         <f aca="false">0.5*B45+0.5*C45</f>
         <v>0.0384306817227434</v>
       </c>
+      <c r="M45" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B45</f>
+        <v>0.000708867860966718</v>
+      </c>
+      <c r="N45" s="8" t="n">
+        <f aca="false">C45-M45</f>
+        <v>0.130717081015873</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="n">
@@ -4252,12 +4707,20 @@
       </c>
       <c r="G46" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B46 + 'Optimal portfolio from homework'!$C$15*C46</f>
-        <v>-0.0835535328685305</v>
+        <v>-0.0835535328685307</v>
       </c>
       <c r="I46" s="1" t="n">
         <f aca="false">0.5*B46+0.5*C46</f>
         <v>-0.0891559721429531</v>
       </c>
+      <c r="M46" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B46</f>
+        <v>-0.00044452143048994</v>
+      </c>
+      <c r="N46" s="8" t="n">
+        <f aca="false">C46-M46</f>
+        <v>-0.107441568383311</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="4" t="n">
@@ -4277,12 +4740,20 @@
       </c>
       <c r="G47" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B47 + 'Optimal portfolio from homework'!$C$15*C47</f>
-        <v>0.0900377339330438</v>
+        <v>0.0900377339330436</v>
       </c>
       <c r="I47" s="1" t="n">
         <f aca="false">0.5*B47+0.5*C47</f>
         <v>0.0818863877872987</v>
       </c>
+      <c r="M47" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B47</f>
+        <v>0.0126128866075064</v>
+      </c>
+      <c r="N47" s="8" t="n">
+        <f aca="false">C47-M47</f>
+        <v>0.0420218586349736</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="4" t="n">
@@ -4308,6 +4779,14 @@
         <f aca="false">0.5*B48+0.5*C48</f>
         <v>-0.00524283063890923</v>
       </c>
+      <c r="M48" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B48</f>
+        <v>0.00450674433373368</v>
+      </c>
+      <c r="N48" s="8" t="n">
+        <f aca="false">C48-M48</f>
+        <v>-0.0126557548110329</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="4" t="n">
@@ -4333,6 +4812,14 @@
         <f aca="false">0.5*B49+0.5*C49</f>
         <v>-0.032910837397847</v>
       </c>
+      <c r="M49" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B49</f>
+        <v>0.00541662939924279</v>
+      </c>
+      <c r="N49" s="8" t="n">
+        <f aca="false">C49-M49</f>
+        <v>-0.0814142819814024</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="4" t="n">
@@ -4352,12 +4839,20 @@
       </c>
       <c r="G50" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B50 + 'Optimal portfolio from homework'!$C$15*C50</f>
-        <v>0.0653909590949816</v>
+        <v>0.0653909590949814</v>
       </c>
       <c r="I50" s="1" t="n">
         <f aca="false">0.5*B50+0.5*C50</f>
         <v>0.0742442154786645</v>
       </c>
+      <c r="M50" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B50</f>
+        <v>0.00792319344944356</v>
+      </c>
+      <c r="N50" s="8" t="n">
+        <f aca="false">C50-M50</f>
+        <v>0.0959192962298194</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="4" t="n">
@@ -4383,6 +4878,14 @@
         <f aca="false">0.5*B51+0.5*C51</f>
         <v>0.0359186145211136</v>
       </c>
+      <c r="M51" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B51</f>
+        <v>0.00780848825289365</v>
+      </c>
+      <c r="N51" s="8" t="n">
+        <f aca="false">C51-M51</f>
+        <v>0.020960211401882</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="4" t="n">
@@ -4402,12 +4905,20 @@
       </c>
       <c r="G52" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B52 + 'Optimal portfolio from homework'!$C$15*C52</f>
-        <v>-0.00362572675978109</v>
+        <v>-0.00362572675978108</v>
       </c>
       <c r="I52" s="1" t="n">
         <f aca="false">0.5*B52+0.5*C52</f>
         <v>-0.0191771769685722</v>
       </c>
+      <c r="M52" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B52</f>
+        <v>0.00706284613910783</v>
+      </c>
+      <c r="N52" s="8" t="n">
+        <f aca="false">C52-M52</f>
+        <v>-0.0782317499422398</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="4" t="n">
@@ -4427,12 +4938,20 @@
       </c>
       <c r="G53" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B53 + 'Optimal portfolio from homework'!$C$15*C53</f>
-        <v>-0.00378492549575952</v>
+        <v>-0.00378492549575953</v>
       </c>
       <c r="I53" s="1" t="n">
         <f aca="false">0.5*B53+0.5*C53</f>
         <v>-0.00267084882725266</v>
       </c>
+      <c r="M53" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B53</f>
+        <v>0.00421160009394802</v>
+      </c>
+      <c r="N53" s="8" t="n">
+        <f aca="false">C53-M53</f>
+        <v>-0.00315785931417986</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="n">
@@ -4458,6 +4977,14 @@
         <f aca="false">0.5*B54+0.5*C54</f>
         <v>-0.0587606104248601</v>
       </c>
+      <c r="M54" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B54</f>
+        <v>0.000293377104218391</v>
+      </c>
+      <c r="N54" s="8" t="n">
+        <f aca="false">C54-M54</f>
+        <v>-0.0575362342470756</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="4" t="n">
@@ -4483,6 +5010,14 @@
         <f aca="false">0.5*B55+0.5*C55</f>
         <v>0.0211827003559973</v>
       </c>
+      <c r="M55" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B55</f>
+        <v>0.00766457731115679</v>
+      </c>
+      <c r="N55" s="8" t="n">
+        <f aca="false">C55-M55</f>
+        <v>-0.00638866024576614</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="4" t="n">
@@ -4508,6 +5043,14 @@
         <f aca="false">0.5*B56+0.5*C56</f>
         <v>0.0238138618875927</v>
       </c>
+      <c r="M56" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B56</f>
+        <v>0.00567286664856078</v>
+      </c>
+      <c r="N56" s="8" t="n">
+        <f aca="false">C56-M56</f>
+        <v>0.0282551359000216</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="n">
@@ -4533,6 +5076,14 @@
         <f aca="false">0.5*B57+0.5*C57</f>
         <v>0.0218808311868364</v>
       </c>
+      <c r="M57" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B57</f>
+        <v>0.00629777152739193</v>
+      </c>
+      <c r="N57" s="8" t="n">
+        <f aca="false">C57-M57</f>
+        <v>0.0151705538462022</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="n">
@@ -4552,12 +5103,20 @@
       </c>
       <c r="G58" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B58 + 'Optimal portfolio from homework'!$C$15*C58</f>
-        <v>0.0426906931104175</v>
+        <v>0.0426906931104174</v>
       </c>
       <c r="I58" s="1" t="n">
         <f aca="false">0.5*B58+0.5*C58</f>
         <v>0.0499565367384358</v>
       </c>
+      <c r="M58" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B58</f>
+        <v>0.00654297264913282</v>
+      </c>
+      <c r="N58" s="8" t="n">
+        <f aca="false">C58-M58</f>
+        <v>0.0677047878696426</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="n">
@@ -4583,6 +5142,14 @@
         <f aca="false">0.5*B59+0.5*C59</f>
         <v>-0.0270842913032633</v>
       </c>
+      <c r="M59" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B59</f>
+        <v>0.00331719437970669</v>
+      </c>
+      <c r="N59" s="8" t="n">
+        <f aca="false">C59-M59</f>
+        <v>-0.038790580118056</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="n">
@@ -4608,6 +5175,14 @@
         <f aca="false">0.5*B60+0.5*C60</f>
         <v>0.00568305853835048</v>
       </c>
+      <c r="M60" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B60</f>
+        <v>0.00507659580825304</v>
+      </c>
+      <c r="N60" s="8" t="n">
+        <f aca="false">C60-M60</f>
+        <v>0.000789644005483973</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="n">
@@ -4627,12 +5202,20 @@
       </c>
       <c r="G61" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B61 + 'Optimal portfolio from homework'!$C$15*C61</f>
-        <v>-0.00726735455217233</v>
+        <v>-0.00726735455217231</v>
       </c>
       <c r="I61" s="1" t="n">
         <f aca="false">0.5*B61+0.5*C61</f>
         <v>-0.0141767594248401</v>
       </c>
+      <c r="M61" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B61</f>
+        <v>0.00532550277809646</v>
+      </c>
+      <c r="N61" s="8" t="n">
+        <f aca="false">C61-M61</f>
+        <v>-0.0426018372204515</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="4" t="n">
@@ -4658,6 +5241,14 @@
         <f aca="false">0.5*B62+0.5*C62</f>
         <v>0.0290361472624296</v>
       </c>
+      <c r="M62" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B62</f>
+        <v>0.00844066873500675</v>
+      </c>
+      <c r="N62" s="8" t="n">
+        <f aca="false">C62-M62</f>
+        <v>-0.00213057258116049</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="4" t="n">
@@ -4677,12 +5268,20 @@
       </c>
       <c r="G63" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B63 + 'Optimal portfolio from homework'!$C$15*C63</f>
-        <v>-0.00877794793035959</v>
+        <v>-0.00877794793035958</v>
       </c>
       <c r="I63" s="1" t="n">
         <f aca="false">0.5*B63+0.5*C63</f>
         <v>-0.0182381642496521</v>
       </c>
+      <c r="M63" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B63</f>
+        <v>0.00565029386324101</v>
+      </c>
+      <c r="N63" s="8" t="n">
+        <f aca="false">C63-M63</f>
+        <v>-0.0555159253950416</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="4" t="n">
@@ -4708,6 +5307,14 @@
         <f aca="false">0.5*B64+0.5*C64</f>
         <v>0.0223073193967138</v>
       </c>
+      <c r="M64" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B64</f>
+        <v>0.00739530476574886</v>
+      </c>
+      <c r="N64" s="8" t="n">
+        <f aca="false">C64-M64</f>
+        <v>-0.000167146374799827</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="4" t="n">
@@ -4733,6 +5340,14 @@
         <f aca="false">0.5*B65+0.5*C65</f>
         <v>-0.0309407108322228</v>
       </c>
+      <c r="M65" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B65</f>
+        <v>0.00606452920726192</v>
+      </c>
+      <c r="N65" s="8" t="n">
+        <f aca="false">C65-M65</f>
+        <v>-0.0870317678968095</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="4" t="n">
@@ -4752,12 +5367,20 @@
       </c>
       <c r="G66" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B66 + 'Optimal portfolio from homework'!$C$15*C66</f>
-        <v>0.000246309478758712</v>
+        <v>0.000246309478758727</v>
       </c>
       <c r="I66" s="1" t="n">
         <f aca="false">0.5*B66+0.5*C66</f>
         <v>-0.00958143303788705</v>
       </c>
+      <c r="M66" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B66</f>
+        <v>0.00636913731569343</v>
+      </c>
+      <c r="N66" s="8" t="n">
+        <f aca="false">C66-M66</f>
+        <v>-0.0488067540191393</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="4" t="n">
@@ -4777,12 +5400,20 @@
       </c>
       <c r="G67" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B67 + 'Optimal portfolio from homework'!$C$15*C67</f>
-        <v>-0.0602115116251324</v>
+        <v>-0.0602115116251322</v>
       </c>
       <c r="I67" s="1" t="n">
         <f aca="false">0.5*B67+0.5*C67</f>
         <v>-0.0801440088325484</v>
       </c>
+      <c r="M67" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B67</f>
+        <v>0.00369457298258859</v>
+      </c>
+      <c r="N67" s="8" t="n">
+        <f aca="false">C67-M67</f>
+        <v>-0.150477058357522</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="4" t="n">
@@ -4802,12 +5433,20 @@
       </c>
       <c r="G68" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B68 + 'Optimal portfolio from homework'!$C$15*C68</f>
-        <v>0.0702997063393526</v>
+        <v>0.0702997063393527</v>
       </c>
       <c r="I68" s="1" t="n">
         <f aca="false">0.5*B68+0.5*C68</f>
         <v>0.0786545043438598</v>
       </c>
+      <c r="M68" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B68</f>
+        <v>0.00836507772393757</v>
+      </c>
+      <c r="N68" s="8" t="n">
+        <f aca="false">C68-M68</f>
+        <v>0.0982212509691854</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="4" t="n">
@@ -4827,12 +5466,20 @@
       </c>
       <c r="G69" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B69 + 'Optimal portfolio from homework'!$C$15*C69</f>
-        <v>-0.00279362796800251</v>
+        <v>-0.0027936279680025</v>
       </c>
       <c r="I69" s="1" t="n">
         <f aca="false">0.5*B69+0.5*C69</f>
         <v>0.00844101317140983</v>
       </c>
+      <c r="M69" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B69</f>
+        <v>0.00255922316455179</v>
+      </c>
+      <c r="N69" s="8" t="n">
+        <f aca="false">C69-M69</f>
+        <v>0.0434415278681181</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="4" t="n">
@@ -4852,12 +5499,20 @@
       </c>
       <c r="G70" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B70 + 'Optimal portfolio from homework'!$C$15*C70</f>
-        <v>0.00593445975970218</v>
+        <v>0.00593445975970219</v>
       </c>
       <c r="I70" s="1" t="n">
         <f aca="false">0.5*B70+0.5*C70</f>
         <v>-0.00485495878938641</v>
       </c>
+      <c r="M70" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B70</f>
+        <v>0.00694662620692531</v>
+      </c>
+      <c r="N70" s="8" t="n">
+        <f aca="false">C70-M70</f>
+        <v>-0.0478728513011633</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="4" t="n">
@@ -4883,6 +5538,14 @@
         <f aca="false">0.5*B71+0.5*C71</f>
         <v>0.0221838817510955</v>
       </c>
+      <c r="M71" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B71</f>
+        <v>0.0080118437687802</v>
+      </c>
+      <c r="N71" s="8" t="n">
+        <f aca="false">C71-M71</f>
+        <v>-0.00950912993759926</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="4" t="n">
@@ -4902,12 +5565,20 @@
       </c>
       <c r="G72" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B72 + 'Optimal portfolio from homework'!$C$15*C72</f>
-        <v>-0.00358198552870319</v>
+        <v>-0.00358198552870321</v>
       </c>
       <c r="I72" s="1" t="n">
         <f aca="false">0.5*B72+0.5*C72</f>
         <v>-0.0180349622825147</v>
       </c>
+      <c r="M72" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B72</f>
+        <v>0.00687885598853995</v>
+      </c>
+      <c r="N72" s="8" t="n">
+        <f aca="false">C72-M72</f>
+        <v>-0.0732331202809487</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="4" t="n">
@@ -4927,12 +5598,20 @@
       </c>
       <c r="G73" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B73 + 'Optimal portfolio from homework'!$C$15*C73</f>
-        <v>0.00401610830444331</v>
+        <v>0.00401610830444333</v>
       </c>
       <c r="I73" s="1" t="n">
         <f aca="false">0.5*B73+0.5*C73</f>
         <v>-0.00499787837563381</v>
       </c>
+      <c r="M73" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B73</f>
+        <v>0.00650460971613832</v>
+      </c>
+      <c r="N73" s="8" t="n">
+        <f aca="false">C73-M73</f>
+        <v>-0.0416381170439841</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="4" t="n">
@@ -4952,12 +5631,20 @@
       </c>
       <c r="G74" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B74 + 'Optimal portfolio from homework'!$C$15*C74</f>
-        <v>-0.00940873093591562</v>
+        <v>-0.00940873093591566</v>
       </c>
       <c r="I74" s="1" t="n">
         <f aca="false">0.5*B74+0.5*C74</f>
         <v>0.00138097072249732</v>
       </c>
+      <c r="M74" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B74</f>
+        <v>0.00215400452393284</v>
+      </c>
+      <c r="N74" s="8" t="n">
+        <f aca="false">C74-M74</f>
+        <v>0.0352991789966665</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="4" t="n">
@@ -4977,12 +5664,20 @@
       </c>
       <c r="G75" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B75 + 'Optimal portfolio from homework'!$C$15*C75</f>
-        <v>0.0524668203756526</v>
+        <v>0.0524668203756527</v>
       </c>
       <c r="I75" s="1" t="n">
         <f aca="false">0.5*B75+0.5*C75</f>
         <v>0.0553945391882922</v>
       </c>
+      <c r="M75" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B75</f>
+        <v>0.00799304762168252</v>
+      </c>
+      <c r="N75" s="8" t="n">
+        <f aca="false">C75-M75</f>
+        <v>0.0571894634092041</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="4" t="n">
@@ -5002,12 +5697,20 @@
       </c>
       <c r="G76" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B76 + 'Optimal portfolio from homework'!$C$15*C76</f>
-        <v>-0.00355686673376058</v>
+        <v>-0.00355686673376057</v>
       </c>
       <c r="I76" s="1" t="n">
         <f aca="false">0.5*B76+0.5*C76</f>
         <v>-0.00859049095799075</v>
       </c>
+      <c r="M76" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B76</f>
+        <v>0.00527570189414656</v>
+      </c>
+      <c r="N76" s="8" t="n">
+        <f aca="false">C76-M76</f>
+        <v>-0.0306946437130131</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="4" t="n">
@@ -5033,6 +5736,14 @@
         <f aca="false">0.5*B77+0.5*C77</f>
         <v>0.00284766241618334</v>
       </c>
+      <c r="M77" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B77</f>
+        <v>0.00520319979641775</v>
+      </c>
+      <c r="N77" s="8" t="n">
+        <f aca="false">C77-M77</f>
+        <v>-0.00674879485051354</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="4" t="n">
@@ -5052,12 +5763,20 @@
       </c>
       <c r="G78" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B78 + 'Optimal portfolio from homework'!$C$15*C78</f>
-        <v>0.00485964118697857</v>
+        <v>0.00485964118697859</v>
       </c>
       <c r="I78" s="1" t="n">
         <f aca="false">0.5*B78+0.5*C78</f>
         <v>-0.0030311641564838</v>
       </c>
+      <c r="M78" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B78</f>
+        <v>0.00637456826586736</v>
+      </c>
+      <c r="N78" s="8" t="n">
+        <f aca="false">C78-M78</f>
+        <v>-0.0357863329717498</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="4" t="n">
@@ -5077,12 +5796,20 @@
       </c>
       <c r="G79" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B79 + 'Optimal portfolio from homework'!$C$15*C79</f>
-        <v>0.0298167420392389</v>
+        <v>0.029816742039239</v>
       </c>
       <c r="I79" s="1" t="n">
         <f aca="false">0.5*B79+0.5*C79</f>
         <v>0.033784477698271</v>
       </c>
+      <c r="M79" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B79</f>
+        <v>0.00616878380910169</v>
+      </c>
+      <c r="N79" s="8" t="n">
+        <f aca="false">C79-M79</f>
+        <v>0.0408806579771822</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="4" t="n">
@@ -5108,6 +5835,14 @@
         <f aca="false">0.5*B80+0.5*C80</f>
         <v>-0.0137947517032299</v>
       </c>
+      <c r="M80" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B80</f>
+        <v>0.00366731067724188</v>
+      </c>
+      <c r="N80" s="8" t="n">
+        <f aca="false">C80-M80</f>
+        <v>-0.0173763738912556</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="4" t="n">
@@ -5133,6 +5868,14 @@
         <f aca="false">0.5*B81+0.5*C81</f>
         <v>0.0163646414151125</v>
       </c>
+      <c r="M81" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B81</f>
+        <v>0.00757605531752216</v>
+      </c>
+      <c r="N81" s="8" t="n">
+        <f aca="false">C81-M81</f>
+        <v>-0.0147189124603793</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="4" t="n">
@@ -5158,6 +5901,14 @@
         <f aca="false">0.5*B82+0.5*C82</f>
         <v>-0.0365473158518247</v>
       </c>
+      <c r="M82" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B82</f>
+        <v>0.00364555645799725</v>
+      </c>
+      <c r="N82" s="8" t="n">
+        <f aca="false">C82-M82</f>
+        <v>-0.062560586596049</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="4" t="n">
@@ -5177,12 +5928,20 @@
       </c>
       <c r="G83" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B83 + 'Optimal portfolio from homework'!$C$15*C83</f>
-        <v>0.00509650890477196</v>
+        <v>0.00509650890477201</v>
       </c>
       <c r="I83" s="1" t="n">
         <f aca="false">0.5*B83+0.5*C83</f>
         <v>-0.00306990008078733</v>
       </c>
+      <c r="M83" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B83</f>
+        <v>0.00643875326371404</v>
+      </c>
+      <c r="N83" s="8" t="n">
+        <f aca="false">C83-M83</f>
+        <v>-0.0368106540901602</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="4" t="n">
@@ -5202,12 +5961,20 @@
       </c>
       <c r="G84" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B84 + 'Optimal portfolio from homework'!$C$15*C84</f>
-        <v>0.0207840487809166</v>
+        <v>0.0207840487809167</v>
       </c>
       <c r="I84" s="1" t="n">
         <f aca="false">0.5*B84+0.5*C84</f>
         <v>0.0182063917678508</v>
       </c>
+      <c r="M84" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B84</f>
+        <v>0.0066272317852837</v>
+      </c>
+      <c r="N84" s="8" t="n">
+        <f aca="false">C84-M84</f>
+        <v>0.00296151741565396</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="4" t="n">
@@ -5227,12 +5994,20 @@
       </c>
       <c r="G85" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B85 + 'Optimal portfolio from homework'!$C$15*C85</f>
-        <v>0.00264685870204491</v>
+        <v>0.0026468587020449</v>
       </c>
       <c r="I85" s="1" t="n">
         <f aca="false">0.5*B85+0.5*C85</f>
         <v>0.00490455710492027</v>
       </c>
+      <c r="M85" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B85</f>
+        <v>0.00448443853712212</v>
+      </c>
+      <c r="N85" s="8" t="n">
+        <f aca="false">C85-M85</f>
+        <v>0.00796807307115128</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="4" t="n">
@@ -5252,12 +6027,20 @@
       </c>
       <c r="G86" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B86 + 'Optimal portfolio from homework'!$C$15*C86</f>
-        <v>-0.000825580114502251</v>
+        <v>-0.000825580114502244</v>
       </c>
       <c r="I86" s="1" t="n">
         <f aca="false">0.5*B86+0.5*C86</f>
         <v>0.0116998932256546</v>
       </c>
+      <c r="M86" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B86</f>
+        <v>0.00248238711492746</v>
+      </c>
+      <c r="N86" s="8" t="n">
+        <f aca="false">C86-M86</f>
+        <v>0.0510927640211992</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="4" t="n">
@@ -5283,6 +6066,14 @@
         <f aca="false">0.5*B87+0.5*C87</f>
         <v>0.00554789120246774</v>
       </c>
+      <c r="M87" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B87</f>
+        <v>0.00885032510221933</v>
+      </c>
+      <c r="N87" s="8" t="n">
+        <f aca="false">C87-M87</f>
+        <v>-0.0551502855296036</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="4" t="n">
@@ -5308,6 +6099,14 @@
         <f aca="false">0.5*B88+0.5*C88</f>
         <v>-0.018652991887949</v>
       </c>
+      <c r="M88" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B88</f>
+        <v>0.00351778572149664</v>
+      </c>
+      <c r="N88" s="8" t="n">
+        <f aca="false">C88-M88</f>
+        <v>-0.0248870803273058</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="4" t="n">
@@ -5333,6 +6132,14 @@
         <f aca="false">0.5*B89+0.5*C89</f>
         <v>0.0153665825061937</v>
       </c>
+      <c r="M89" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B89</f>
+        <v>0.00536680872781189</v>
+      </c>
+      <c r="N89" s="8" t="n">
+        <f aca="false">C89-M89</f>
+        <v>0.015875506302928</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="4" t="n">
@@ -5352,12 +6159,20 @@
       </c>
       <c r="G90" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B90 + 'Optimal portfolio from homework'!$C$15*C90</f>
-        <v>0.00422142531998363</v>
+        <v>0.00422142531998362</v>
       </c>
       <c r="I90" s="1" t="n">
         <f aca="false">0.5*B90+0.5*C90</f>
         <v>0.000591987979771725</v>
       </c>
+      <c r="M90" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B90</f>
+        <v>0.00560205663536702</v>
+      </c>
+      <c r="N90" s="8" t="n">
+        <f aca="false">C90-M90</f>
+        <v>-0.0171440312264157</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="4" t="n">
@@ -5383,6 +6198,14 @@
         <f aca="false">0.5*B91+0.5*C91</f>
         <v>-0.0161329988197073</v>
       </c>
+      <c r="M91" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B91</f>
+        <v>0.00327109356311064</v>
+      </c>
+      <c r="N91" s="8" t="n">
+        <f aca="false">C91-M91</f>
+        <v>-0.0162079215201</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="4" t="n">
@@ -5402,12 +6225,20 @@
       </c>
       <c r="G92" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B92 + 'Optimal portfolio from homework'!$C$15*C92</f>
-        <v>-0.0148062473179306</v>
+        <v>-0.0148062473179305</v>
       </c>
       <c r="I92" s="1" t="n">
         <f aca="false">0.5*B92+0.5*C92</f>
         <v>-0.0300029104988085</v>
       </c>
+      <c r="M92" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B92</f>
+        <v>0.00618937561674631</v>
+      </c>
+      <c r="N92" s="8" t="n">
+        <f aca="false">C92-M92</f>
+        <v>-0.0869978862550442</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="4" t="n">
@@ -5433,6 +6264,14 @@
         <f aca="false">0.5*B93+0.5*C93</f>
         <v>-0.00916721192691372</v>
       </c>
+      <c r="M93" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B93</f>
+        <v>0.000283382449951282</v>
+      </c>
+      <c r="N93" s="8" t="n">
+        <f aca="false">C93-M93</f>
+        <v>0.041798002671108</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="4" t="n">
@@ -5458,6 +6297,14 @@
         <f aca="false">0.5*B94+0.5*C94</f>
         <v>-0.0137829130177405</v>
       </c>
+      <c r="M94" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B94</f>
+        <v>0.00286597258483837</v>
+      </c>
+      <c r="N94" s="8" t="n">
+        <f aca="false">C94-M94</f>
+        <v>-0.00553145459283481</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="4" t="n">
@@ -5483,6 +6330,14 @@
         <f aca="false">0.5*B95+0.5*C95</f>
         <v>0.0533607985127715</v>
       </c>
+      <c r="M95" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B95</f>
+        <v>0.0108014347436044</v>
+      </c>
+      <c r="N95" s="8" t="n">
+        <f aca="false">C95-M95</f>
+        <v>0.011692997327665</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="4" t="n">
@@ -5508,6 +6363,14 @@
         <f aca="false">0.5*B96+0.5*C96</f>
         <v>-0.0386901335672687</v>
       </c>
+      <c r="M96" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B96</f>
+        <v>0.00488489916900052</v>
+      </c>
+      <c r="N96" s="8" t="n">
+        <f aca="false">C96-M96</f>
+        <v>-0.0851288547342367</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="4" t="n">
@@ -5527,12 +6390,20 @@
       </c>
       <c r="G97" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B97 + 'Optimal portfolio from homework'!$C$15*C97</f>
-        <v>-0.00825375926240242</v>
+        <v>-0.0082537592624024</v>
       </c>
       <c r="I97" s="1" t="n">
         <f aca="false">0.5*B97+0.5*C97</f>
         <v>-0.00493689469892684</v>
       </c>
+      <c r="M97" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B97</f>
+        <v>0.00351130134099577</v>
+      </c>
+      <c r="N97" s="8" t="n">
+        <f aca="false">C97-M97</f>
+        <v>0.00264077084201927</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="4" t="n">
@@ -5552,12 +6423,20 @@
       </c>
       <c r="G98" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B98 + 'Optimal portfolio from homework'!$C$15*C98</f>
-        <v>-0.0157164545466873</v>
+        <v>-0.0157164545466874</v>
       </c>
       <c r="I98" s="1" t="n">
         <f aca="false">0.5*B98+0.5*C98</f>
         <v>-0.00114237299818061</v>
       </c>
+      <c r="M98" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B98</f>
+        <v>0.00105049624701459</v>
+      </c>
+      <c r="N98" s="8" t="n">
+        <f aca="false">C98-M98</f>
+        <v>0.0465313112370995</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="4" t="n">
@@ -5577,12 +6456,20 @@
       </c>
       <c r="G99" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B99 + 'Optimal portfolio from homework'!$C$15*C99</f>
-        <v>0.037037661122522</v>
+        <v>0.0370376611225219</v>
       </c>
       <c r="I99" s="1" t="n">
         <f aca="false">0.5*B99+0.5*C99</f>
         <v>0.0535489440994973</v>
       </c>
+      <c r="M99" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B99</f>
+        <v>0.00455655191869472</v>
+      </c>
+      <c r="N99" s="8" t="n">
+        <f aca="false">C99-M99</f>
+        <v>0.10419303923954</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="4" t="n">
@@ -5608,6 +6495,14 @@
         <f aca="false">0.5*B100+0.5*C100</f>
         <v>0.0334543624796803</v>
       </c>
+      <c r="M100" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B100</f>
+        <v>0.00958903386913442</v>
+      </c>
+      <c r="N100" s="8" t="n">
+        <f aca="false">C100-M100</f>
+        <v>-0.0102346847219482</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="4" t="n">
@@ -5633,6 +6528,14 @@
         <f aca="false">0.5*B101+0.5*C101</f>
         <v>0.0183460161532155</v>
       </c>
+      <c r="M101" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B101</f>
+        <v>0.00494113515001932</v>
+      </c>
+      <c r="N101" s="8" t="n">
+        <f aca="false">C101-M101</f>
+        <v>0.0281138583648965</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="4" t="n">
@@ -5652,12 +6555,20 @@
       </c>
       <c r="G102" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B102 + 'Optimal portfolio from homework'!$C$15*C102</f>
-        <v>-0.00611678268076337</v>
+        <v>-0.00611678268076332</v>
       </c>
       <c r="I102" s="1" t="n">
         <f aca="false">0.5*B102+0.5*C102</f>
         <v>-0.0162933600126559</v>
       </c>
+      <c r="M102" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B102</f>
+        <v>0.00596586878130342</v>
+      </c>
+      <c r="N102" s="8" t="n">
+        <f aca="false">C102-M102</f>
+        <v>-0.0562816396718487</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="4" t="n">
@@ -5677,12 +6588,20 @@
       </c>
       <c r="G103" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B103 + 'Optimal portfolio from homework'!$C$15*C103</f>
-        <v>0.0322557058959493</v>
+        <v>0.0322557058959492</v>
       </c>
       <c r="I103" s="1" t="n">
         <f aca="false">0.5*B103+0.5*C103</f>
         <v>0.0450399134330096</v>
       </c>
+      <c r="M103" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B103</f>
+        <v>0.00484388404081549</v>
+      </c>
+      <c r="N103" s="8" t="n">
+        <f aca="false">C103-M103</f>
+        <v>0.0829362894412167</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="4" t="n">
@@ -5708,6 +6627,14 @@
         <f aca="false">0.5*B104+0.5*C104</f>
         <v>0.0240663696267819</v>
       </c>
+      <c r="M104" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B104</f>
+        <v>0.00733546468434142</v>
+      </c>
+      <c r="N104" s="8" t="n">
+        <f aca="false">C104-M104</f>
+        <v>0.00423370767708608</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="4" t="n">
@@ -5727,12 +6654,20 @@
       </c>
       <c r="G105" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B105 + 'Optimal portfolio from homework'!$C$15*C105</f>
-        <v>-0.004105987747718</v>
+        <v>-0.00410598774771798</v>
       </c>
       <c r="I105" s="1" t="n">
         <f aca="false">0.5*B105+0.5*C105</f>
         <v>-0.0063255405127233</v>
       </c>
+      <c r="M105" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B105</f>
+        <v>0.00475627650357791</v>
+      </c>
+      <c r="N105" s="8" t="n">
+        <f aca="false">C105-M105</f>
+        <v>-0.0185022427324709</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="4" t="n">
@@ -5752,12 +6687,20 @@
       </c>
       <c r="G106" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B106 + 'Optimal portfolio from homework'!$C$15*C106</f>
-        <v>0.00343902244732037</v>
+        <v>0.00343902244732038</v>
       </c>
       <c r="I106" s="1" t="n">
         <f aca="false">0.5*B106+0.5*C106</f>
         <v>0.00495711569318677</v>
       </c>
+      <c r="M106" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B106</f>
+        <v>0.0046680652497776</v>
+      </c>
+      <c r="N106" s="8" t="n">
+        <f aca="false">C106-M106</f>
+        <v>0.0053643513503213</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="4" t="n">
@@ -5783,6 +6726,14 @@
         <f aca="false">0.5*B107+0.5*C107</f>
         <v>-0.0295852724313393</v>
       </c>
+      <c r="M107" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B107</f>
+        <v>0.00332915232147005</v>
+      </c>
+      <c r="N107" s="8" t="n">
+        <f aca="false">C107-M107</f>
+        <v>-0.0439689444744937</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="4" t="n">
@@ -5802,12 +6753,20 @@
       </c>
       <c r="G108" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B108 + 'Optimal portfolio from homework'!$C$15*C108</f>
-        <v>5.44733669617485E-005</v>
+        <v>5.4473366961804E-005</v>
       </c>
       <c r="I108" s="1" t="n">
         <f aca="false">0.5*B108+0.5*C108</f>
         <v>-0.0156656241775686</v>
       </c>
+      <c r="M108" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B108</f>
+        <v>0.00735919662977047</v>
+      </c>
+      <c r="N108" s="8" t="n">
+        <f aca="false">C108-M108</f>
+        <v>-0.0755803706997751</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="4" t="n">
@@ -5827,12 +6786,20 @@
       </c>
       <c r="G109" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B109 + 'Optimal portfolio from homework'!$C$15*C109</f>
-        <v>0.00409601288114885</v>
+        <v>0.00409601288114881</v>
       </c>
       <c r="I109" s="1" t="n">
         <f aca="false">0.5*B109+0.5*C109</f>
         <v>-0.0024036991610871</v>
       </c>
+      <c r="M109" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B109</f>
+        <v>0.00608200832070421</v>
+      </c>
+      <c r="N109" s="8" t="n">
+        <f aca="false">C109-M109</f>
+        <v>-0.0302155943068927</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="4" t="n">
@@ -5858,6 +6825,14 @@
         <f aca="false">0.5*B110+0.5*C110</f>
         <v>0.0261410503172827</v>
       </c>
+      <c r="M110" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B110</f>
+        <v>0.00601694093308875</v>
+      </c>
+      <c r="N110" s="8" t="n">
+        <f aca="false">C110-M110</f>
+        <v>0.0278337708260347</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="4" t="n">
@@ -5883,6 +6858,14 @@
         <f aca="false">0.5*B111+0.5*C111</f>
         <v>0.0415608884756657</v>
       </c>
+      <c r="M111" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B111</f>
+        <v>0.0075291775523777</v>
+      </c>
+      <c r="N111" s="8" t="n">
+        <f aca="false">C111-M111</f>
+        <v>0.0363651167419166</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="4" t="n">
@@ -5908,6 +6891,14 @@
         <f aca="false">0.5*B112+0.5*C112</f>
         <v>-0.00387355766354112</v>
       </c>
+      <c r="M112" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B112</f>
+        <v>0.00472759788231224</v>
+      </c>
+      <c r="N112" s="8" t="n">
+        <f aca="false">C112-M112</f>
+        <v>-0.0131752135065634</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="4" t="n">
@@ -5927,12 +6918,20 @@
       </c>
       <c r="G113" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B113 + 'Optimal portfolio from homework'!$C$15*C113</f>
-        <v>0.0128443855060477</v>
+        <v>0.0128443855060476</v>
       </c>
       <c r="I113" s="1" t="n">
         <f aca="false">0.5*B113+0.5*C113</f>
         <v>0.0141943445823999</v>
       </c>
+      <c r="M113" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B113</f>
+        <v>0.00538064691979305</v>
+      </c>
+      <c r="N113" s="8" t="n">
+        <f aca="false">C113-M113</f>
+        <v>0.0133268911328767</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="4" t="n">
@@ -5952,12 +6951,20 @@
       </c>
       <c r="G114" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B114 + 'Optimal portfolio from homework'!$C$15*C114</f>
-        <v>0.00796856963868845</v>
+        <v>0.00796856963868843</v>
       </c>
       <c r="I114" s="1" t="n">
         <f aca="false">0.5*B114+0.5*C114</f>
         <v>0.00567732121053493</v>
       </c>
+      <c r="M114" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B114</f>
+        <v>0.00564652255158847</v>
+      </c>
+      <c r="N114" s="8" t="n">
+        <f aca="false">C114-M114</f>
+        <v>-0.00762932054455595</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="4" t="n">
@@ -5977,12 +6984,20 @@
       </c>
       <c r="G115" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B115 + 'Optimal portfolio from homework'!$C$15*C115</f>
-        <v>-0.00232582466775868</v>
+        <v>-0.00232582466775865</v>
       </c>
       <c r="I115" s="1" t="n">
         <f aca="false">0.5*B115+0.5*C115</f>
         <v>-0.00567235121195071</v>
       </c>
+      <c r="M115" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B115</f>
+        <v>0.0050777523460549</v>
+      </c>
+      <c r="N115" s="8" t="n">
+        <f aca="false">C115-M115</f>
+        <v>-0.0219382365998925</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="4" t="n">
@@ -6008,6 +7023,14 @@
         <f aca="false">0.5*B116+0.5*C116</f>
         <v>0.0188024574040601</v>
       </c>
+      <c r="M116" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B116</f>
+        <v>0.00611097842472152</v>
+      </c>
+      <c r="N116" s="8" t="n">
+        <f aca="false">C116-M116</f>
+        <v>0.0117693553778122</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="4" t="n">
@@ -6033,6 +7056,14 @@
         <f aca="false">0.5*B117+0.5*C117</f>
         <v>0.0161435014495335</v>
       </c>
+      <c r="M117" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B117</f>
+        <v>0.00482460118689389</v>
+      </c>
+      <c r="N117" s="8" t="n">
+        <f aca="false">C117-M117</f>
+        <v>0.0254279237864547</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="4" t="n">
@@ -6052,12 +7083,20 @@
       </c>
       <c r="G118" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B118 + 'Optimal portfolio from homework'!$C$15*C118</f>
-        <v>0.00741608245127781</v>
+        <v>0.0074160824512778</v>
       </c>
       <c r="I118" s="1" t="n">
         <f aca="false">0.5*B118+0.5*C118</f>
         <v>0.00217763209815781</v>
       </c>
+      <c r="M118" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B118</f>
+        <v>0.00610852626718476</v>
+      </c>
+      <c r="N118" s="8" t="n">
+        <f aca="false">C118-M118</f>
+        <v>-0.0214441213047096</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="4" t="n">
@@ -6083,6 +7122,14 @@
         <f aca="false">0.5*B119+0.5*C119</f>
         <v>0.00581203971324846</v>
       </c>
+      <c r="M119" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B119</f>
+        <v>0.00629649759472925</v>
+      </c>
+      <c r="N119" s="8" t="n">
+        <f aca="false">C119-M119</f>
+        <v>-0.0169482362015128</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="4" t="n">
@@ -6108,6 +7155,14 @@
         <f aca="false">0.5*B120+0.5*C120</f>
         <v>0.0175373350978611</v>
       </c>
+      <c r="M120" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B120</f>
+        <v>0.00684315448780895</v>
+      </c>
+      <c r="N120" s="8" t="n">
+        <f aca="false">C120-M120</f>
+        <v>-0.0015618613302445</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="4" t="n">
@@ -6133,6 +7188,14 @@
         <f aca="false">0.5*B121+0.5*C121</f>
         <v>0.0102060107709963</v>
       </c>
+      <c r="M121" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B121</f>
+        <v>0.00541255036007012</v>
+      </c>
+      <c r="N121" s="8" t="n">
+        <f aca="false">C121-M121</f>
+        <v>0.00487958784528798</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="4" t="n">
@@ -6152,12 +7215,20 @@
       </c>
       <c r="G122" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B122 + 'Optimal portfolio from homework'!$C$15*C122</f>
-        <v>0.0485705360748743</v>
+        <v>0.0485705360748742</v>
       </c>
       <c r="I122" s="1" t="n">
         <f aca="false">0.5*B122+0.5*C122</f>
         <v>0.0454312005485714</v>
       </c>
+      <c r="M122" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B122</f>
+        <v>0.00874349665221516</v>
+      </c>
+      <c r="N122" s="8" t="n">
+        <f aca="false">C122-M122</f>
+        <v>0.0261922534441982</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="4" t="n">
@@ -6183,6 +7254,14 @@
         <f aca="false">0.5*B123+0.5*C123</f>
         <v>-0.0281715561870194</v>
       </c>
+      <c r="M123" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B123</f>
+        <v>0.00190725464696532</v>
+      </c>
+      <c r="N123" s="8" t="n">
+        <f aca="false">C123-M123</f>
+        <v>-0.0201658506941607</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="4" t="n">
@@ -6208,6 +7287,14 @@
         <f aca="false">0.5*B124+0.5*C124</f>
         <v>-0.0124943088211856</v>
       </c>
+      <c r="M124" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B124</f>
+        <v>0.00274126768091882</v>
+      </c>
+      <c r="N124" s="8" t="n">
+        <f aca="false">C124-M124</f>
+        <v>-0.00111461464751724</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="4" t="n">
@@ -6233,6 +7320,14 @@
         <f aca="false">0.5*B125+0.5*C125</f>
         <v>-0.00242298373394866</v>
       </c>
+      <c r="M125" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B125</f>
+        <v>0.0048462663482131</v>
+      </c>
+      <c r="N125" s="8" t="n">
+        <f aca="false">C125-M125</f>
+        <v>-0.0120246484012383</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="4" t="n">
@@ -6258,6 +7353,14 @@
         <f aca="false">0.5*B126+0.5*C126</f>
         <v>0.00572956210667881</v>
       </c>
+      <c r="M126" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B126</f>
+        <v>0.00631612515854089</v>
+      </c>
+      <c r="N126" s="8" t="n">
+        <f aca="false">C126-M126</f>
+        <v>-0.0174027348451506</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="4" t="n">
@@ -6283,6 +7386,14 @@
         <f aca="false">0.5*B127+0.5*C127</f>
         <v>-0.0186854312139832</v>
       </c>
+      <c r="M127" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B127</f>
+        <v>0.0050148343698003</v>
+      </c>
+      <c r="N127" s="8" t="n">
+        <f aca="false">C127-M127</f>
+        <v>-0.0470362382823435</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="4" t="n">
@@ -6308,6 +7419,14 @@
         <f aca="false">0.5*B128+0.5*C128</f>
         <v>0.00441207081299066</v>
       </c>
+      <c r="M128" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B128</f>
+        <v>0.00725762399973959</v>
+      </c>
+      <c r="N128" s="8" t="n">
+        <f aca="false">C128-M128</f>
+        <v>-0.0339265936530921</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="4" t="n">
@@ -6333,6 +7452,14 @@
         <f aca="false">0.5*B129+0.5*C129</f>
         <v>0.0095664750217545</v>
       </c>
+      <c r="M129" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B129</f>
+        <v>0.00692090140837504</v>
+      </c>
+      <c r="N129" s="8" t="n">
+        <f aca="false">C129-M129</f>
+        <v>-0.0186504945842282</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="4" t="n">
@@ -6352,12 +7479,20 @@
       </c>
       <c r="G130" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B130 + 'Optimal portfolio from homework'!$C$15*C130</f>
-        <v>-0.00467951430744668</v>
+        <v>-0.00467951430744665</v>
       </c>
       <c r="I130" s="1" t="n">
         <f aca="false">0.5*B130+0.5*C130</f>
         <v>-0.00840219492540467</v>
       </c>
+      <c r="M130" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B130</f>
+        <v>0.00497069187564996</v>
+      </c>
+      <c r="N130" s="8" t="n">
+        <f aca="false">C130-M130</f>
+        <v>-0.0258185810085164</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="4" t="n">
@@ -6383,6 +7518,14 @@
         <f aca="false">0.5*B131+0.5*C131</f>
         <v>-0.0216963789236417</v>
       </c>
+      <c r="M131" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B131</f>
+        <v>-0.000441921187723923</v>
+      </c>
+      <c r="N131" s="8" t="n">
+        <f aca="false">C131-M131</f>
+        <v>0.0274392595907657</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="4" t="n">
@@ -6402,12 +7545,20 @@
       </c>
       <c r="G132" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B132 + 'Optimal portfolio from homework'!$C$15*C132</f>
-        <v>0.0121556691074828</v>
+        <v>0.0121556691074827</v>
       </c>
       <c r="I132" s="1" t="n">
         <f aca="false">0.5*B132+0.5*C132</f>
         <v>0.00946242618313312</v>
       </c>
+      <c r="M132" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B132</f>
+        <v>0.00601949386247403</v>
+      </c>
+      <c r="N132" s="8" t="n">
+        <f aca="false">C132-M132</f>
+        <v>-0.00556113794558154</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="4" t="n">
@@ -6433,6 +7584,14 @@
         <f aca="false">0.5*B133+0.5*C133</f>
         <v>-0.0221279896405985</v>
       </c>
+      <c r="M133" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B133</f>
+        <v>-0.00204252591139982</v>
+      </c>
+      <c r="N133" s="8" t="n">
+        <f aca="false">C133-M133</f>
+        <v>0.0501879640694562</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="4" t="n">
@@ -6458,6 +7617,14 @@
         <f aca="false">0.5*B134+0.5*C134</f>
         <v>0.0538468579790604</v>
       </c>
+      <c r="M134" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B134</f>
+        <v>0.010342848276288</v>
+      </c>
+      <c r="N134" s="8" t="n">
+        <f aca="false">C134-M134</f>
+        <v>0.0194301279652755</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="4" t="n">
@@ -6477,12 +7644,20 @@
       </c>
       <c r="G135" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B135 + 'Optimal portfolio from homework'!$C$15*C135</f>
-        <v>0.0197708558587252</v>
+        <v>0.0197708558587253</v>
       </c>
       <c r="I135" s="1" t="n">
         <f aca="false">0.5*B135+0.5*C135</f>
         <v>0.0153178723189283</v>
       </c>
+      <c r="M135" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B135</f>
+        <v>0.00687309540028002</v>
+      </c>
+      <c r="N135" s="8" t="n">
+        <f aca="false">C135-M135</f>
+        <v>-0.00644247158175456</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="4" t="n">
@@ -6502,12 +7677,20 @@
       </c>
       <c r="G136" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B136 + 'Optimal portfolio from homework'!$C$15*C136</f>
-        <v>0.00161079682321437</v>
+        <v>0.00161079682321438</v>
       </c>
       <c r="I136" s="1" t="n">
         <f aca="false">0.5*B136+0.5*C136</f>
         <v>-0.00515581511289069</v>
       </c>
+      <c r="M136" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B136</f>
+        <v>0.0059467675799588</v>
+      </c>
+      <c r="N136" s="8" t="n">
+        <f aca="false">C136-M136</f>
+        <v>-0.0337247712768165</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="4" t="n">
@@ -6533,6 +7716,14 @@
         <f aca="false">0.5*B137+0.5*C137</f>
         <v>0.0157821788940825</v>
       </c>
+      <c r="M137" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B137</f>
+        <v>0.0074625608504326</v>
+      </c>
+      <c r="N137" s="8" t="n">
+        <f aca="false">C137-M137</f>
+        <v>-0.0142095809487945</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="4" t="n">
@@ -6558,6 +7749,14 @@
         <f aca="false">0.5*B138+0.5*C138</f>
         <v>-0.029701728634898</v>
       </c>
+      <c r="M138" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B138</f>
+        <v>-0.000104218608704321</v>
+      </c>
+      <c r="N138" s="8" t="n">
+        <f aca="false">C138-M138</f>
+        <v>0.00644681285840272</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="4" t="n">
@@ -6583,6 +7782,14 @@
         <f aca="false">0.5*B139+0.5*C139</f>
         <v>0.078580675502476</v>
       </c>
+      <c r="M139" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B139</f>
+        <v>0.00965992428962377</v>
+      </c>
+      <c r="N139" s="8" t="n">
+        <f aca="false">C139-M139</f>
+        <v>0.0789721744758083</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="4" t="n">
@@ -6608,6 +7815,14 @@
         <f aca="false">0.5*B140+0.5*C140</f>
         <v>0.0113679859785599</v>
       </c>
+      <c r="M140" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B140</f>
+        <v>0.00557536353921074</v>
+      </c>
+      <c r="N140" s="8" t="n">
+        <f aca="false">C140-M140</f>
+        <v>0.00480173807414887</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="4" t="n">
@@ -6627,12 +7842,20 @@
       </c>
       <c r="G141" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B141 + 'Optimal portfolio from homework'!$C$15*C141</f>
-        <v>0.0115820523818305</v>
+        <v>0.0115820523818304</v>
       </c>
       <c r="I141" s="1" t="n">
         <f aca="false">0.5*B141+0.5*C141</f>
         <v>0.0239979921818742</v>
       </c>
+      <c r="M141" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B141</f>
+        <v>0.0034033007638098</v>
+      </c>
+      <c r="N141" s="8" t="n">
+        <f aca="false">C141-M141</f>
+        <v>0.062103755962624</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="4" t="n">
@@ -6652,12 +7875,20 @@
       </c>
       <c r="G142" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B142 + 'Optimal portfolio from homework'!$C$15*C142</f>
-        <v>0.00133271077060091</v>
+        <v>0.00133271077060093</v>
       </c>
       <c r="I142" s="1" t="n">
         <f aca="false">0.5*B142+0.5*C142</f>
         <v>-0.00526328084577746</v>
       </c>
+      <c r="M142" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B142</f>
+        <v>0.00589747359432712</v>
+      </c>
+      <c r="N142" s="8" t="n">
+        <f aca="false">C142-M142</f>
+        <v>-0.033212523871095</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="4" t="n">
@@ -6677,12 +7908,20 @@
       </c>
       <c r="G143" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B143 + 'Optimal portfolio from homework'!$C$15*C143</f>
-        <v>0.0168267824955331</v>
+        <v>0.0168267824955332</v>
       </c>
       <c r="I143" s="1" t="n">
         <f aca="false">0.5*B143+0.5*C143</f>
         <v>0.0154939020208448</v>
       </c>
+      <c r="M143" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B143</f>
+        <v>0.0061273701619964</v>
+      </c>
+      <c r="N143" s="8" t="n">
+        <f aca="false">C143-M143</f>
+        <v>0.0049104356997945</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="4" t="n">
@@ -6708,6 +7947,14 @@
         <f aca="false">0.5*B144+0.5*C144</f>
         <v>0.000289673824706887</v>
       </c>
+      <c r="M144" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B144</f>
+        <v>0.00722207565063412</v>
+      </c>
+      <c r="N144" s="8" t="n">
+        <f aca="false">C144-M144</f>
+        <v>-0.0416469827138312</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="4" t="n">
@@ -6733,6 +7980,14 @@
         <f aca="false">0.5*B145+0.5*C145</f>
         <v>0.0365098909784005</v>
       </c>
+      <c r="M145" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B145</f>
+        <v>0.00676035177959754</v>
+      </c>
+      <c r="N145" s="8" t="n">
+        <f aca="false">C145-M145</f>
+        <v>0.0376047458960988</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="4" t="n">
@@ -6758,6 +8013,14 @@
         <f aca="false">0.5*B146+0.5*C146</f>
         <v>0.0174405780183681</v>
       </c>
+      <c r="M146" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B146</f>
+        <v>0.00454554377636636</v>
+      </c>
+      <c r="N146" s="8" t="n">
+        <f aca="false">C146-M146</f>
+        <v>0.0321386978519988</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="4" t="n">
@@ -6783,6 +8046,14 @@
         <f aca="false">0.5*B147+0.5*C147</f>
         <v>-0.0280156787293362</v>
       </c>
+      <c r="M147" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B147</f>
+        <v>-0.00140348043090416</v>
+      </c>
+      <c r="N147" s="8" t="n">
+        <f aca="false">C147-M147</f>
+        <v>0.0289854648063984</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="4" t="n">
@@ -6802,12 +8073,20 @@
       </c>
       <c r="G148" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B148 + 'Optimal portfolio from homework'!$C$15*C148</f>
-        <v>-0.0863396661308425</v>
+        <v>-0.0863396661308423</v>
       </c>
       <c r="I148" s="1" t="n">
         <f aca="false">0.5*B148+0.5*C148</f>
         <v>-0.0698318426484181</v>
       </c>
+      <c r="M148" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B148</f>
+        <v>-0.00441452964868975</v>
+      </c>
+      <c r="N148" s="8" t="n">
+        <f aca="false">C148-M148</f>
+        <v>-0.0102282317495331</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="4" t="n">
@@ -6827,12 +8106,20 @@
       </c>
       <c r="G149" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B149 + 'Optimal portfolio from homework'!$C$15*C149</f>
-        <v>0.107715015136304</v>
+        <v>0.107715015136305</v>
       </c>
       <c r="I149" s="1" t="n">
         <f aca="false">0.5*B149+0.5*C149</f>
         <v>0.0989989813799583</v>
       </c>
+      <c r="M149" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B149</f>
+        <v>0.0139945496250109</v>
+      </c>
+      <c r="N149" s="8" t="n">
+        <f aca="false">C149-M149</f>
+        <v>0.0558649212876492</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="4" t="n">
@@ -6858,6 +8145,14 @@
         <f aca="false">0.5*B150+0.5*C150</f>
         <v>0.0262529751290291</v>
       </c>
+      <c r="M150" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B150</f>
+        <v>0.00812504185031593</v>
+      </c>
+      <c r="N150" s="8" t="n">
+        <f aca="false">C150-M150</f>
+        <v>-0.00304082749178959</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="4" t="n">
@@ -6883,6 +8178,14 @@
         <f aca="false">0.5*B151+0.5*C151</f>
         <v>0.0228596311840037</v>
       </c>
+      <c r="M151" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B151</f>
+        <v>0.00611014773211471</v>
+      </c>
+      <c r="N151" s="8" t="n">
+        <f aca="false">C151-M151</f>
+        <v>0.0198959572138476</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="4" t="n">
@@ -6902,12 +8205,20 @@
       </c>
       <c r="G152" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B152 + 'Optimal portfolio from homework'!$C$15*C152</f>
-        <v>0.0768247103761605</v>
+        <v>0.0768247103761603</v>
       </c>
       <c r="I152" s="1" t="n">
         <f aca="false">0.5*B152+0.5*C152</f>
         <v>0.0856393854992584</v>
       </c>
+      <c r="M152" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B152</f>
+        <v>0.00876119935863425</v>
+      </c>
+      <c r="N152" s="8" t="n">
+        <f aca="false">C152-M152</f>
+        <v>0.10634747517686</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="4" t="n">
@@ -6933,6 +8244,14 @@
         <f aca="false">0.5*B153+0.5*C153</f>
         <v>0.031011578140065</v>
       </c>
+      <c r="M153" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B153</f>
+        <v>0.00988823185480264</v>
+      </c>
+      <c r="N153" s="8" t="n">
+        <f aca="false">C153-M153</f>
+        <v>-0.0195339856401878</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="4" t="n">
@@ -6952,12 +8271,20 @@
       </c>
       <c r="G154" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B154 + 'Optimal portfolio from homework'!$C$15*C154</f>
-        <v>-0.0378331800899039</v>
+        <v>-0.0378331800899038</v>
       </c>
       <c r="I154" s="1" t="n">
         <f aca="false">0.5*B154+0.5*C154</f>
         <v>-0.0376742049382362</v>
       </c>
+      <c r="M154" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B154</f>
+        <v>0.00189844308332901</v>
+      </c>
+      <c r="N154" s="8" t="n">
+        <f aca="false">C154-M154</f>
+        <v>-0.0390411610831755</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="4" t="n">
@@ -6983,6 +8310,14 @@
         <f aca="false">0.5*B155+0.5*C155</f>
         <v>-0.0154743769615043</v>
       </c>
+      <c r="M155" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B155</f>
+        <v>0.00272685307839545</v>
+      </c>
+      <c r="N155" s="8" t="n">
+        <f aca="false">C155-M155</f>
+        <v>-0.00686210846758526</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="4" t="n">
@@ -7002,12 +8337,20 @@
       </c>
       <c r="G156" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B156 + 'Optimal portfolio from homework'!$C$15*C156</f>
-        <v>0.0515316033020503</v>
+        <v>0.0515316033020505</v>
       </c>
       <c r="I156" s="1" t="n">
         <f aca="false">0.5*B156+0.5*C156</f>
         <v>0.0268966657690494</v>
       </c>
+      <c r="M156" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B156</f>
+        <v>0.0126214924361148</v>
+      </c>
+      <c r="N156" s="8" t="n">
+        <f aca="false">C156-M156</f>
+        <v>-0.0680845375368718</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="4" t="n">
@@ -7033,6 +8376,14 @@
         <f aca="false">0.5*B157+0.5*C157</f>
         <v>0.0527158800236891</v>
       </c>
+      <c r="M157" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B157</f>
+        <v>0.00746096677611144</v>
+      </c>
+      <c r="N157" s="8" t="n">
+        <f aca="false">C157-M157</f>
+        <v>0.0596813369006288</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="4" t="n">
@@ -7058,6 +8409,14 @@
         <f aca="false">0.5*B158+0.5*C158</f>
         <v>-0.0153595724077338</v>
       </c>
+      <c r="M158" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B158</f>
+        <v>0.00392668889065666</v>
+      </c>
+      <c r="N158" s="8" t="n">
+        <f aca="false">C158-M158</f>
+        <v>-0.0243323311094711</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="4" t="n">
@@ -7077,12 +8436,20 @@
       </c>
       <c r="G159" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B159 + 'Optimal portfolio from homework'!$C$15*C159</f>
-        <v>0.00132305922127853</v>
+        <v>0.00132305922127852</v>
       </c>
       <c r="I159" s="1" t="n">
         <f aca="false">0.5*B159+0.5*C159</f>
         <v>-0.00986807142777518</v>
       </c>
+      <c r="M159" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B159</f>
+        <v>0.00667974588451348</v>
+      </c>
+      <c r="N159" s="8" t="n">
+        <f aca="false">C159-M159</f>
+        <v>-0.0539620905706473</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="4" t="n">
@@ -7102,12 +8469,20 @@
       </c>
       <c r="G160" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B160 + 'Optimal portfolio from homework'!$C$15*C160</f>
-        <v>0.0125536387375484</v>
+        <v>0.0125536387375485</v>
       </c>
       <c r="I160" s="1" t="n">
         <f aca="false">0.5*B160+0.5*C160</f>
         <v>-0.000739581368041593</v>
       </c>
+      <c r="M160" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B160</f>
+        <v>0.00785458261050906</v>
+      </c>
+      <c r="N160" s="8" t="n">
+        <f aca="false">C160-M160</f>
+        <v>-0.0530361587251769</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="4" t="n">
@@ -7133,6 +8508,14 @@
         <f aca="false">0.5*B161+0.5*C161</f>
         <v>0.0513710537012719</v>
       </c>
+      <c r="M161" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B161</f>
+        <v>0.00854719756411066</v>
+      </c>
+      <c r="N161" s="8" t="n">
+        <f aca="false">C161-M161</f>
+        <v>0.0409677399859532</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="4" t="n">
@@ -7158,6 +8541,14 @@
         <f aca="false">0.5*B162+0.5*C162</f>
         <v>0.0383834962434079</v>
       </c>
+      <c r="M162" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B162</f>
+        <v>0.00517556150168541</v>
+      </c>
+      <c r="N162" s="8" t="n">
+        <f aca="false">C162-M162</f>
+        <v>0.0647305895611822</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="4" t="n">
@@ -7183,6 +8574,14 @@
         <f aca="false">0.5*B163+0.5*C163</f>
         <v>-0.0239592005245571</v>
       </c>
+      <c r="M163" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B163</f>
+        <v>0.00636608330305026</v>
+      </c>
+      <c r="N163" s="8" t="n">
+        <f aca="false">C163-M163</f>
+        <v>-0.0775172365699794</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="4" t="n">
@@ -7208,6 +8607,14 @@
         <f aca="false">0.5*B164+0.5*C164</f>
         <v>0.0318491855509627</v>
       </c>
+      <c r="M164" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B164</f>
+        <v>0.00639423303313414</v>
+      </c>
+      <c r="N164" s="8" t="n">
+        <f aca="false">C164-M164</f>
+        <v>0.0336842741918062</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="4" t="n">
@@ -7233,6 +8640,14 @@
         <f aca="false">0.5*B165+0.5*C165</f>
         <v>0.0113300482624552</v>
       </c>
+      <c r="M165" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B165</f>
+        <v>0.0068792926054073</v>
+      </c>
+      <c r="N165" s="8" t="n">
+        <f aca="false">C165-M165</f>
+        <v>-0.0145095401098515</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="4" t="n">
@@ -7258,6 +8673,14 @@
         <f aca="false">0.5*B166+0.5*C166</f>
         <v>-0.0462857533506754</v>
       </c>
+      <c r="M166" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B166</f>
+        <v>0.00128578264787129</v>
+      </c>
+      <c r="N166" s="8" t="n">
+        <f aca="false">C166-M166</f>
+        <v>-0.0472263657928859</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="4" t="n">
@@ -7283,6 +8706,14 @@
         <f aca="false">0.5*B167+0.5*C167</f>
         <v>0.0538430952865217</v>
       </c>
+      <c r="M167" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B167</f>
+        <v>0.00976195426071061</v>
+      </c>
+      <c r="N167" s="8" t="n">
+        <f aca="false">C167-M167</f>
+        <v>0.0279918803387868</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="4" t="n">
@@ -7308,6 +8739,14 @@
         <f aca="false">0.5*B168+0.5*C168</f>
         <v>-0.00316357517846211</v>
       </c>
+      <c r="M168" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B168</f>
+        <v>0.00416393956629807</v>
+      </c>
+      <c r="N168" s="8" t="n">
+        <f aca="false">C168-M168</f>
+        <v>-0.00344022971827723</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="4" t="n">
@@ -7327,12 +8766,20 @@
       </c>
       <c r="G169" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B169 + 'Optimal portfolio from homework'!$C$15*C169</f>
-        <v>0.033312376527198</v>
+        <v>0.0333123765271981</v>
       </c>
       <c r="I169" s="1" t="n">
         <f aca="false">0.5*B169+0.5*C169</f>
         <v>0.028501257778436</v>
       </c>
+      <c r="M169" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B169</f>
+        <v>0.00791882207275415</v>
+      </c>
+      <c r="N169" s="8" t="n">
+        <f aca="false">C169-M169</f>
+        <v>0.00449786684580405</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="4" t="n">
@@ -7358,6 +8805,14 @@
         <f aca="false">0.5*B170+0.5*C170</f>
         <v>-0.0340326549202227</v>
       </c>
+      <c r="M170" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B170</f>
+        <v>0.000905726516815402</v>
+      </c>
+      <c r="N170" s="8" t="n">
+        <f aca="false">C170-M170</f>
+        <v>-0.017113627181614</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="4" t="n">
@@ -7377,12 +8832,20 @@
       </c>
       <c r="G171" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B171 + 'Optimal portfolio from homework'!$C$15*C171</f>
-        <v>0.00257244027110335</v>
+        <v>0.00257244027110332</v>
       </c>
       <c r="I171" s="1" t="n">
         <f aca="false">0.5*B171+0.5*C171</f>
         <v>0.0164716967036144</v>
       </c>
+      <c r="M171" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B171</f>
+        <v>0.00249540071011792</v>
+      </c>
+      <c r="N171" s="8" t="n">
+        <f aca="false">C171-M171</f>
+        <v>0.0604443960060665</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="4" t="n">
@@ -7408,6 +8871,14 @@
         <f aca="false">0.5*B172+0.5*C172</f>
         <v>0.0238307074103138</v>
       </c>
+      <c r="M172" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B172</f>
+        <v>0.00735505912717684</v>
+      </c>
+      <c r="N172" s="8" t="n">
+        <f aca="false">C172-M172</f>
+        <v>0.00347332841025806</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="4" t="n">
@@ -7433,6 +8904,14 @@
         <f aca="false">0.5*B173+0.5*C173</f>
         <v>-0.0459991671524006</v>
       </c>
+      <c r="M173" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B173</f>
+        <v>-0.00167903436485816</v>
+      </c>
+      <c r="N173" s="8" t="n">
+        <f aca="false">C173-M173</f>
+        <v>-0.00291657397150682</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="4" t="n">
@@ -7458,6 +8937,14 @@
         <f aca="false">0.5*B174+0.5*C174</f>
         <v>-0.0153847266520647</v>
       </c>
+      <c r="M174" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B174</f>
+        <v>0.00477867834936455</v>
+      </c>
+      <c r="N174" s="8" t="n">
+        <f aca="false">C174-M174</f>
+        <v>-0.03695108431141</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="4" t="n">
@@ -7483,6 +8970,14 @@
         <f aca="false">0.5*B175+0.5*C175</f>
         <v>-0.0529279006129414</v>
       </c>
+      <c r="M175" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B175</f>
+        <v>-0.00137735554607881</v>
+      </c>
+      <c r="N175" s="8" t="n">
+        <f aca="false">C175-M175</f>
+        <v>-0.0212243700794606</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="4" t="n">
@@ -7508,6 +9003,14 @@
         <f aca="false">0.5*B176+0.5*C176</f>
         <v>0.0301672333814152</v>
       </c>
+      <c r="M176" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B176</f>
+        <v>0.0113154232654484</v>
+      </c>
+      <c r="N176" s="8" t="n">
+        <f aca="false">C176-M176</f>
+        <v>-0.0422764289998991</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="4" t="n">
@@ -7533,6 +9036,14 @@
         <f aca="false">0.5*B177+0.5*C177</f>
         <v>-0.0355718431259389</v>
       </c>
+      <c r="M177" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B177</f>
+        <v>0.00156386938688653</v>
+      </c>
+      <c r="N177" s="8" t="n">
+        <f aca="false">C177-M177</f>
+        <v>-0.0299008470433764</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="4" t="n">
@@ -7558,6 +9069,14 @@
         <f aca="false">0.5*B178+0.5*C178</f>
         <v>-0.059577999858666</v>
       </c>
+      <c r="M178" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B178</f>
+        <v>-0.00216614142686536</v>
+      </c>
+      <c r="N178" s="8" t="n">
+        <f aca="false">C178-M178</f>
+        <v>-0.0228884953402451</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="4" t="n">
@@ -7583,6 +9102,14 @@
         <f aca="false">0.5*B179+0.5*C179</f>
         <v>0.0279731627823729</v>
       </c>
+      <c r="M179" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B179</f>
+        <v>0.0103858689338464</v>
+      </c>
+      <c r="N179" s="8" t="n">
+        <f aca="false">C179-M179</f>
+        <v>-0.0329518979280177</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="4" t="n">
@@ -7602,12 +9129,20 @@
       </c>
       <c r="G180" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B180 + 'Optimal portfolio from homework'!$C$15*C180</f>
-        <v>0.0591478993384031</v>
+        <v>0.0591478993384032</v>
       </c>
       <c r="I180" s="1" t="n">
         <f aca="false">0.5*B180+0.5*C180</f>
         <v>0.0618330862590725</v>
       </c>
+      <c r="M180" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B180</f>
+        <v>0.00852020336290738</v>
+      </c>
+      <c r="N180" s="8" t="n">
+        <f aca="false">C180-M180</f>
+        <v>0.0622900202695178</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="4" t="n">
@@ -7633,6 +9168,14 @@
         <f aca="false">0.5*B181+0.5*C181</f>
         <v>-0.0171887830262654</v>
       </c>
+      <c r="M181" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B181</f>
+        <v>0.00023895981314226</v>
+      </c>
+      <c r="N181" s="8" t="n">
+        <f aca="false">C181-M181</f>
+        <v>0.026410177799451</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="4" t="n">
@@ -7658,6 +9201,14 @@
         <f aca="false">0.5*B182+0.5*C182</f>
         <v>0.0534567945386652</v>
       </c>
+      <c r="M182" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B182</f>
+        <v>0.00898019973739931</v>
+      </c>
+      <c r="N182" s="8" t="n">
+        <f aca="false">C182-M182</f>
+        <v>0.0387516263447594</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="4" t="n">
@@ -7683,6 +9234,14 @@
         <f aca="false">0.5*B183+0.5*C183</f>
         <v>-0.0405803508627402</v>
       </c>
+      <c r="M183" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B183</f>
+        <v>0.0026480513475353</v>
+      </c>
+      <c r="N183" s="8" t="n">
+        <f aca="false">C183-M183</f>
+        <v>-0.0559115827353161</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="4" t="n">
@@ -7702,12 +9261,20 @@
       </c>
       <c r="G184" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B184 + 'Optimal portfolio from homework'!$C$15*C184</f>
-        <v>0.0527962012377525</v>
+        <v>0.0527962012377524</v>
       </c>
       <c r="I184" s="1" t="n">
         <f aca="false">0.5*B184+0.5*C184</f>
         <v>0.0612560036837277</v>
       </c>
+      <c r="M184" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B184</f>
+        <v>0.00707437749631474</v>
+      </c>
+      <c r="N184" s="8" t="n">
+        <f aca="false">C184-M184</f>
+        <v>0.0824645021854884</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="4" t="n">
@@ -7727,12 +9294,20 @@
       </c>
       <c r="G185" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B185 + 'Optimal portfolio from homework'!$C$15*C185</f>
-        <v>0.00726478899066119</v>
+        <v>0.0072647889906612</v>
       </c>
       <c r="I185" s="1" t="n">
         <f aca="false">0.5*B185+0.5*C185</f>
         <v>0.00524004177353027</v>
       </c>
+      <c r="M185" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B185</f>
+        <v>0.00554993586734992</v>
+      </c>
+      <c r="N185" s="8" t="n">
+        <f aca="false">C185-M185</f>
+        <v>-0.00707904441798668</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="4" t="n">
@@ -7752,12 +9327,20 @@
       </c>
       <c r="G186" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B186 + 'Optimal portfolio from homework'!$C$15*C186</f>
-        <v>-0.00505585486408199</v>
+        <v>-0.00505585486408198</v>
       </c>
       <c r="I186" s="1" t="n">
         <f aca="false">0.5*B186+0.5*C186</f>
         <v>-0.00747285698285578</v>
       </c>
+      <c r="M186" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B186</f>
+        <v>0.00472084844935728</v>
+      </c>
+      <c r="N186" s="8" t="n">
+        <f aca="false">C186-M186</f>
+        <v>-0.0202742453323956</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="4" t="n">
@@ -7777,12 +9360,20 @@
       </c>
       <c r="G187" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B187 + 'Optimal portfolio from homework'!$C$15*C187</f>
-        <v>0.0289204536956684</v>
+        <v>0.0289204536956685</v>
       </c>
       <c r="I187" s="1" t="n">
         <f aca="false">0.5*B187+0.5*C187</f>
         <v>0.0148235656714074</v>
       </c>
+      <c r="M187" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B187</f>
+        <v>0.0091816722994831</v>
+      </c>
+      <c r="N187" s="8" t="n">
+        <f aca="false">C187-M187</f>
+        <v>-0.0414869300840671</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="4" t="n">
@@ -7808,6 +9399,14 @@
         <f aca="false">0.5*B188+0.5*C188</f>
         <v>0.0251706719309951</v>
       </c>
+      <c r="M188" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B188</f>
+        <v>0.0066781287488941</v>
+      </c>
+      <c r="N188" s="8" t="n">
+        <f aca="false">C188-M188</f>
+        <v>0.0161392519345658</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="4" t="n">
@@ -7833,6 +9432,14 @@
         <f aca="false">0.5*B189+0.5*C189</f>
         <v>-0.0154132291238179</v>
       </c>
+      <c r="M189" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B189</f>
+        <v>0.00318432033930414</v>
+      </c>
+      <c r="N189" s="8" t="n">
+        <f aca="false">C189-M189</f>
+        <v>-0.01348831410065</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="4" t="n">
@@ -7858,6 +9465,14 @@
         <f aca="false">0.5*B190+0.5*C190</f>
         <v>-0.046862476759159</v>
       </c>
+      <c r="M190" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B190</f>
+        <v>0.00088931369814251</v>
+      </c>
+      <c r="N190" s="8" t="n">
+        <f aca="false">C190-M190</f>
+        <v>-0.0425311509576838</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="4" t="n">
@@ -7877,12 +9492,20 @@
       </c>
       <c r="G191" s="1" t="n">
         <f aca="false">'Optimal portfolio from homework'!$B$15*B191 + 'Optimal portfolio from homework'!$C$15*C191</f>
-        <v>0.00515182989980938</v>
+        <v>0.00515182989980935</v>
       </c>
       <c r="I191" s="1" t="n">
         <f aca="false">0.5*B191+0.5*C191</f>
         <v>0.0183840427019796</v>
       </c>
+      <c r="M191" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B191</f>
+        <v>0.00279662584380418</v>
+      </c>
+      <c r="N191" s="8" t="n">
+        <f aca="false">C191-M191</f>
+        <v>0.0598254515231545</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="4" t="n">
@@ -7908,6 +9531,14 @@
         <f aca="false">0.5*B192+0.5*C192</f>
         <v>0.0512723173669493</v>
       </c>
+      <c r="M192" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B192</f>
+        <v>0.0109881940160097</v>
+      </c>
+      <c r="N192" s="8" t="n">
+        <f aca="false">C192-M192</f>
+        <v>0.00476098499880811</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="4" t="n">
@@ -7932,6 +9563,14 @@
       <c r="I193" s="1" t="n">
         <f aca="false">0.5*B193+0.5*C193</f>
         <v>0.0281533054034589</v>
+      </c>
+      <c r="M193" s="1" t="n">
+        <f aca="false">'Optimal portfolio from homework'!D$34+'Optimal portfolio from homework'!D$32*B193</f>
+        <v>0.007658260556139</v>
+      </c>
+      <c r="N193" s="8" t="n">
+        <f aca="false">C193-M193</f>
+        <v>0.00764573384973</v>
       </c>
     </row>
   </sheetData>
@@ -7946,36 +9585,36 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1048576"/>
+  <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E38" activeCellId="0" sqref="E38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E32" activeCellId="0" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="29.03"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="1" t="n">
@@ -7988,146 +9627,146 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="8" t="n">
+      <c r="B4" s="6" t="n">
         <f aca="false">STDEV('Excess returns'!B2:B193)</f>
         <v>0.0468841732364885</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="6" t="n">
         <f aca="false">STDEV('Excess returns'!C2:C193)</f>
         <v>0.049457764779768</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="9" t="n">
+      <c r="B5" s="10" t="n">
         <f aca="false">B3/B4</f>
         <v>0.173489773832912</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <f aca="false">C3/C4</f>
         <v>0.106517889515185</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="9" t="n">
+      <c r="B6" s="10" t="n">
         <f aca="false">CORREL('Excess returns'!B2:B193,'Excess returns'!C2:C193)</f>
         <v>0.0689334096375325</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
+      <c r="A9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="5" t="n">
         <f aca="false">B4^2</f>
         <v>0.00219812570006906</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="5" t="n">
         <f aca="false">B4*C4*B6</f>
         <v>0.000159841853588218</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="10" t="n">
+      <c r="B12" s="11" t="n">
         <f aca="false">B4*C4*B6</f>
         <v>0.000159841853588218</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="5" t="n">
         <f aca="false">C4^2</f>
         <v>0.00244607049701086</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="10" t="n">
-        <f aca="false" t="array" ref="B14:C14"> TRANSPOSE( MMULT( MINVERSE( B11:C12 ), TRANSPOSE( B3:C3 ) ) )</f>
-        <v>3.5606984382885</v>
-      </c>
-      <c r="C14" s="0" t="n">
+      <c r="B14" s="11" t="n">
+        <f aca="false" t="array" ref="B14:C14">TRANSPOSE( MMULT( MINVERSE( B11:C12 ), TRANSPOSE( B3:C3 ) ) )</f>
+        <v>3.56069843828851</v>
+      </c>
+      <c r="C14" s="5" t="n">
         <v>1.92103542877316</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B15" s="1" t="n">
         <f aca="false">B14/(B14+C14)</f>
-        <v>0.64955696949898</v>
+        <v>0.649556969498981</v>
       </c>
       <c r="C15" s="1" t="n">
         <f aca="false">C14/(B14+C14)</f>
-        <v>0.35044303050102</v>
+        <v>0.350443030501019</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="12" t="n">
         <f aca="false">MMULT(B15:C15,TRANSPOSE(B3:C3)) / SQRT( MMULT( B15:C15, MMULT( B11:C12, TRANSPOSE(B15:C15) ) ) )</f>
         <v>0.197693525314801</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
+      <c r="A20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="0" t="s">
+      <c r="J21" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="1" t="n">
@@ -8148,174 +9787,174 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D23" s="1" t="n">
         <f aca="false">B4</f>
         <v>0.0468841732364885</v>
       </c>
-      <c r="F23" s="8" t="n">
+      <c r="F23" s="6" t="n">
         <f aca="false">STDEV('Excess returns'!E2:E193)</f>
         <v>0.039443537633849</v>
       </c>
-      <c r="H23" s="8" t="n">
+      <c r="H23" s="6" t="n">
         <f aca="false">STDEV('Excess returns'!G2:G193)</f>
-        <v>0.0360640501908876</v>
-      </c>
-      <c r="J23" s="8" t="n">
+        <v>0.0360640501908877</v>
+      </c>
+      <c r="J23" s="6" t="n">
         <f aca="false">STDEV('Excess returns'!I2:I193)</f>
         <v>0.0352274037655926</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="9" t="n">
+      <c r="B24" s="10" t="n">
         <f aca="false">C5</f>
         <v>0.106517889515185</v>
       </c>
-      <c r="D24" s="9" t="n">
+      <c r="D24" s="10" t="n">
         <f aca="false">B5</f>
         <v>0.173489773832912</v>
       </c>
-      <c r="F24" s="9" t="n">
+      <c r="F24" s="10" t="n">
         <f aca="false">F22/F23</f>
         <v>0.191685824532145</v>
       </c>
-      <c r="H24" s="9" t="n">
+      <c r="H24" s="10" t="n">
         <f aca="false">H22/H23</f>
-        <v>0.197693525314801</v>
-      </c>
-      <c r="J24" s="9" t="n">
+        <v>0.1976935253148</v>
+      </c>
+      <c r="J24" s="10" t="n">
         <f aca="false">J22/J23</f>
         <v>0.190222098466293</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D25" s="9" t="n">
+      <c r="D25" s="10" t="n">
         <f aca="false">B6</f>
         <v>0.0689334096375325</v>
       </c>
-      <c r="F25" s="9" t="n">
+      <c r="F25" s="10" t="n">
         <f aca="false">CORREL('Excess returns'!E2:E193,'Excess returns'!C2:C193)</f>
         <v>0.316327146088148</v>
       </c>
-      <c r="H25" s="9" t="n">
+      <c r="H25" s="10" t="n">
         <f aca="false">CORREL('Excess returns'!G2:G193,'Excess returns'!$C2:$C193)</f>
         <v>0.538803126433047</v>
       </c>
-      <c r="J25" s="9" t="n">
+      <c r="J25" s="10" t="n">
         <f aca="false">CORREL('Excess returns'!I2:I193,'Excess returns'!$C2:$C193)</f>
         <v>0.747850324843681</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="9" t="n">
+      <c r="D26" s="10" t="n">
         <f aca="false">D24*D25</f>
         <v>0.011959241647547</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9" t="n">
+      <c r="E26" s="10"/>
+      <c r="F26" s="10" t="n">
         <f aca="false">F24*F25</f>
         <v>0.060635429819807</v>
       </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="9" t="n">
+      <c r="G26" s="10"/>
+      <c r="H26" s="10" t="n">
         <f aca="false">H24*H25</f>
         <v>0.106517889515185</v>
       </c>
-      <c r="J26" s="9" t="n">
+      <c r="J26" s="10" t="n">
         <f aca="false">J24*J25</f>
         <v>0.142257658130464</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6" t="s">
+      <c r="E27" s="7"/>
+      <c r="F27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="6" t="s">
+      <c r="J27" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="0" t="s">
+      <c r="D31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="0" t="s">
+      <c r="F31" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H31" s="0" t="s">
+      <c r="H31" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J31" s="0" t="s">
+      <c r="J31" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="9" t="n">
+      <c r="D32" s="10" t="n">
         <f aca="false">B6*C4/B4</f>
         <v>0.0727173398605893</v>
       </c>
-      <c r="F32" s="9" t="n">
+      <c r="F32" s="10" t="n">
         <f aca="false">F25*C4/F23</f>
         <v>0.396638702388021</v>
       </c>
-      <c r="H32" s="9" t="n">
+      <c r="H32" s="10" t="n">
         <f aca="false">H25*C4/H23</f>
         <v>0.738907531147525</v>
       </c>
-      <c r="J32" s="9" t="n">
+      <c r="J32" s="10" t="n">
         <f aca="false">J25*C4/J23</f>
         <v>1.0499497976833</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="9" t="n">
+      <c r="D33" s="10" t="n">
         <f aca="false">SLOPE('Excess returns'!C2:C193,'Excess returns'!B2:B193)</f>
         <v>0.0727173398605893</v>
       </c>
-      <c r="F33" s="9" t="n">
+      <c r="F33" s="10" t="n">
         <f aca="false">SLOPE('Excess returns'!C2:C193,'Excess returns'!E2:E193)</f>
         <v>0.39663870238802</v>
       </c>
-      <c r="H33" s="9" t="n">
+      <c r="H33" s="10" t="n">
         <f aca="false">SLOPE('Excess returns'!C2:C193,'Excess returns'!G2:G193)</f>
-        <v>0.738907531147525</v>
-      </c>
-      <c r="J33" s="9" t="n">
+        <v>0.738907531147524</v>
+      </c>
+      <c r="J33" s="10" t="n">
         <f aca="false">SLOPE('Excess returns'!C2:C193,'Excess returns'!I2:I193)</f>
         <v>1.0499497976833</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D34" s="1" t="n">
@@ -8336,57 +9975,57 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="8" t="n">
+      <c r="D35" s="6" t="n">
         <f aca="false">INTERCEPT('Excess returns'!C2:C193,'Excess returns'!B2:B193)</f>
         <v>0.00467665936413056</v>
       </c>
-      <c r="F35" s="8" t="n">
+      <c r="F35" s="6" t="n">
         <f aca="false">INTERCEPT('Excess returns'!C2:C193,'Excess returns'!E2:E193)</f>
         <v>0.00226924389913121</v>
       </c>
-      <c r="H35" s="8" t="n">
+      <c r="H35" s="6" t="n">
         <f aca="false">INTERCEPT('Excess returns'!C2:C193,'Excess returns'!G2:G193)</f>
-        <v>8.67361737988404E-019</v>
-      </c>
-      <c r="J35" s="8" t="n">
+        <v>8.67361737988404E-018</v>
+      </c>
+      <c r="J35" s="6" t="n">
         <f aca="false">INTERCEPT('Excess returns'!C2:C193,'Excess returns'!I2:I193)</f>
         <v>-0.00176760906945777</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D36" s="6" t="s">
+      <c r="D36" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6" t="s">
+      <c r="E36" s="7"/>
+      <c r="F36" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6" t="s">
+      <c r="G36" s="7"/>
+      <c r="H36" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J36" s="6" t="s">
+      <c r="J36" s="7" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="6" t="s">
+      <c r="A40" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="6"/>
+      <c r="A41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D42" s="13" t="n">
@@ -8395,39 +10034,47 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="9" t="n">
+      <c r="D43" s="13" t="n">
+        <f aca="false">STDEV('Excess returns'!N2:N193)</f>
+        <v>0.0493401177807627</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="10" t="n">
         <f aca="false">D35/D42</f>
         <v>0.0947841143166859</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D44" s="9" t="n">
-        <f aca="false">SQRT(D43^2 + B5^2)</f>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="10" t="n">
+        <f aca="false">SQRT(D44^2 + B5^2)</f>
         <v>0.197693525314801</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+      <c r="A47" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>